<commit_message>
added verification of cellphone number and id number
</commit_message>
<xml_diff>
--- a/declarationTable.xlsx
+++ b/declarationTable.xlsx
@@ -66,6 +66,74 @@
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -358,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -411,260 +479,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2020_9_20_10:36</t>
+          <t>2020_9_20_11:31</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>l</t>
+          <t>אלכס</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>l</t>
+          <t>0526354845</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>l</t>
+          <t>22</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>כן</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>כן</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>כן</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wBDAAMCAgICAgMCAgIDAwMDBAYEBAQEBAgGBgUGCQgKCgkICQkKDA8MCgsOCwkJDRENDg8QEBEQCgwSExIQEw8QEBD/2wBDAQMDAwQDBAgEBAgQCwkLEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBD/wAARCAEzATMDASIAAhEBAxEB/8QAGwABAAIDAQEAAAAAAAAAAAAAAAgJBQYHBAL/xAA2EAEAAgEDAwMCAwYEBwAAAAAAAQIDBAURBgcICRIhEzEUQVEiIzIzQmEVFnFyGBlic4GSof/EABQBAQAAAAAAAAAAAAAAAAAAAAD/xAAUEQEAAAAAAAAAAAAAAAAAAAAA/9oADAMBAAIRAxEAPwC1MAAAAAAAAAAAAAAAAAAAAAAc06x8mPHjt/8AUp1n3v6H2nNi93u0+ffdN+I5r/FEYYvOSZj9IrLhPXHqueG/SGW+l2nrDeur9XSYrGn6f2bNkm9pn4rS+o+ljtP2+15j5+/IJgiDv/Mq6y3vF+I6B8Fu+O/4b0x5cWWdmy46Xpf5i3OLFliKzHzE8zEvnH5heenVcxi6L9PPctsva0Vrbfeoq4q888cz9XFp+I+Y/P4+Z54BOQQdx9c+rp1DH7nsz2X6Wx2tSYjWa7JqMtI4+YtbFrMlZjn9K8/bjn5lksGn9WzPbnJr/HvTxEfbJG4TE8R/01mfnn/4CaAh3ixerFhvOC+q8b88XmKxmvG7RGOPj9riIiePv+U/afj7MXu/Tnq5Y/fq9F192Dy+60caXR4dZ+zHH5Tm00fHx+dvzBNgV25t49Z/atJ+O/yx293W2G9rzpaW0EZMtazM8fzaRxMRxHFotxMc8Ty1rpn1bu5PbbrTS9A+XPjpqultTN4rrdbt1c+my6fHPMRmro9RFpzU90fxUzfaJmvuniJCzcYTovrTpfuJ0rtvW3RW84N22PeMEanQ63Bz7M2OZmPdHuiJj5iY4mIn4ZsAAAAAAAAAAAAAAAAAAAAAAB4923fadh2/Nu2+bppNu0Onr7s2p1eeuHFjj9bXtMREf6yg35u+oluPabqvePG3sZ0NvW+908mCumnV00v1MW321GlrmxZNNipF76rNWmWt4rNYpExzPviJqrq0/i96gvk7vddb1R0J3J3nPxGSuu6yzZtHhpSY5icd9dakTXifiMfPx9oBbb3B9SHw07dZ8mi3DvPt286vHPH0dg0+bcot/pmw1th/t/McN6n9arx026LY+le3fXu85ax8Wz4NJo8Np+Ptb617/r96flH355jjfaT0TOrNdfBr++Hdvb9qwcxbJt3TeC2qzWr8c1nUZq0pjtxzHxjyRz+qdvZXwO8W+xGDFk6S7W7buW647Vv/AIxv2Ou4673xHHupfLE1wz/2q0j+wImaXzT9QryorX/hY8eMHR/T2f4p1Buta6iPjiJtTU6qMemtEfMzSuLJb7ff8/TpvTO8oO9M11/lX5gbvq8eaffl2basufWYaxP3rX6tsWHFPzxMUw2r+nMLKwELeg/SN8O+kIx33zYuo+sc9Ji033reb0rNv9mkjDXj+08/aOefnmS/bvsR2W7S0pHbTtX0t01lpWafiNu2vDi1F4nnn35or9S/xPHNrT8fDewAAAAAABxTy+8cti8nOyG/9v8AWbfoLb7XTX1PTuv1OKJvodwrEWxzW/xNK3msY7zE/NbTzE8cO1gKwvRy74b1ordY+KXW1s+DW9O5c28bRp9TeffpojLGLXaWKz/D7ctq5PbH9WTNP6rPVQ3ROCvbD1q9x2nSzfTaXeN619s+OvtrGT/ENovqoiYj44+tlpb9fiPzW8gAAAAAAAAAAAAAAAAAAAAAA12nbnt7j6zydxsfQfTterMuKMGTfq7Xgjcb44pFIpOp9v1Zr7YivHu44jj7NiAAAAAAAAAAAAAAAFR3lBp69G+sJ253ylZxz1Bu3S2S1qVrM3nLauh5nj+2Pj5+eI/ThbirA83Nmwa/1U/HSZ9kzfT9PZrV+0+7BvGsyRaeJ5n+GP8A1/P7LPwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAVxd8MUb/wCsh2Y27Wzj+loOlovi9/HHOPDuuor/AOff9v78LHVcXlDp67L6s3j9vum+nF9x2TBpstePmZ+tuGObTP6+zJER/tWOgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAro9WHpfqHt/1D2k8v+iNsy5tz6A3jFpNxzVtaaRhjNXPpYyRFZiuOcn18c2mfmc9a8TzHE5Ozndfpbvl2y6f7sdFV1tNl6j006nS01uGMWox8XtS9MlYm0Rat6WrPttas8cxMxMTOteVfZy3f3x5647T4c1sWr3vbZtobRMRH4zBeufTxbn49s5sWOJ/tM/aeJVq+nT55YfHbLm8ZPJCu47Js+m3C+La9w1+K9LbDqL2/eaXVY7RFseGck2t7uP3dr390e2fdQLgh59v3Hb930Gn3Xatdp9botZirn0+p0+WuTFmx2jmt6XrMxasxMTExPExL0AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAIxeXHp/wDZvyxpO/bp9XpfrbDijFg6j27DW98taxxWmqwzMRqKRHxH7VbxxEReK81mToCpPa/FT1NfC7PafHzrbD1t0rW1s99t0Wpx5cPtiYmYvt+s49l7/nOmm15j+qGbp6wHfDthFdh79+J19LveKYpltGs1Wyfr8/Q1ODNPM8T/AF8TxK1EBofYnuth74do+me7Gn6c1+w4+pNH+Lrt2u/nYI99qcTPEe6J9vurbiPdW1Z/NvgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA//2Q==</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2020_9_20_10:37</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>,</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>,</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>,</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wBDAAMCAgICAgMCAgIDAwMDBAYEBAQEBAgGBgUGCQgKCgkICQkKDA8MCgsOCwkJDRENDg8QEBEQCgwSExIQEw8QEBD/2wBDAQMDAwQDBAgEBAgQCwkLEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBD/wAARCAEzATMDASIAAhEBAxEB/8QAGgABAAMBAQEAAAAAAAAAAAAAAAYHCQgFA//EADQQAQABAwQCAQIFAgMJAAAAAAABAgMEBQYHEQgSIQkxEyIjMkEUURUXQxYzQlJicZGSof/EABQBAQAAAAAAAAAAAAAAAAAAAAD/xAAUEQEAAAAAAAAAAAAAAAAAAAAA/9oADAMBAAIRAxEAPwDVMAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAHNPmd5saP4b0bKydb481LcuJu7Ky7N29iZdNiMKjHizNU/moqi5XVF7umjunv0q/NHQOlhGuOeR9k8tbM0zkDjvcOLreg6vai9i5ePV8T/emqmeqqK6Z7iqiqIqpmJiYiYSUAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABGOSeNNj8vbL1Pj7kXb2NrWhatam1k4t+P/WuiqPzUV0z8010zFVMxExMJOAyC17avkT9JXlC5u7ZdzN3vwhuDLpjKx71U02p9p6i3f8AWJpxsuKYiKL8U+lyIiJifm3TplwF5D8W+SmxMffvF24Lebj1RTRm4VyYozNOvz33ZyLXczRV8T1PzTVEe1M1UzEp3uDb2hbs0TN23ufR8PVdK1KzVj5eFmWabtm/bq+9NdFUTFUf92YXOvhlzV4S79v+THhFqWfkbes93db2rNVeRXZx/b2qtTa77y8T7/E/q2uoqiZ696Q1NHO3iB5scX+W+1ou6Hfo0beOBYpr1jbeRd7vWJ+03bNXUfjWJn7VxHcdxFcUzMd9EgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA4N8svpw17h3N/n/4k6v/ALB8n4F+c+vExMj+kxNSvfM1V26o+Me/V3MT/pXO+q4p9qq5jHBf1RtR2Tr08Nec2zdQ2RuzTZjHua7Tp9cWL0x3EV5OPRE1W/bqOrtmK7VXfcRRT8tGVc80ePHDHkJolvQeXtg6duCzj9zjX7kVWsrFmfv+FkW5pu24n+YiqInqO4noEs2jvTaG/wDQrG59jbo0rcGkZP8Auc7TMy3k2K5j7xFdEzHcd/MfeP5e0y75G+nx5F+KG5bnLPgXyLreZiU/qZ22crJtzk3KKe5mmaaopsZtvrvqiumLlPx6+9XUxanjD9UPQt/7x/yc8k9n08Xb6tV04dN3KquWcLKy++ps10XoivDuT3HrTcqqpq+3vEzTTUHeAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAADmjzF8FOLfLXQ6s7ULcaDvnBx5taXuLGo7q6juabOTR9r1nv8Av1XT8+tUd1RV0uAyj8WvNfkbw337k+J3mlGoW9L0m5Tj6Tr12a8qvTrU9fhd1/uv4NVPzRXTE1W/29esetvU7RNb0bcukYev7e1XE1LTNQs05GJmYl6m7Zv2qo7prorpmYqiY/mFX+Sfi3xP5SbJu7S5H0Sicuzbr/wrWseiKc7TLsx8V2q/5p769rdXdFXXzHcRMZubD5J8kvpSci2eM+WtPubt4g13LqnBzLVdf4FFPf5r+HVPt+DdiJiq7jVRPt18fui5IbAjydq7q23vnbenbv2hrWJq+i6vj0ZWFm4tyK7V+1VHcVUzH/iY+8TExPUw9YAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABXvPXCOzPIbjDWOLt8YsV4WpWpmxfij2rw8mKZi1kUR3H5qJq7j5+fmP5WEAxa4u5h8jPpT8q3eLOZNCydw8eav+Jfs42Jf9sXIjuO8zTr1cR61xMxFyzV69+0e8UzNFbXzjDkvZ3MOwtF5K2DqtOoaFr2NTlYt6I6qjv4qt10/wDDcoqiaaqZ+YqpmP4RfyO8eNg+TfGGo8Z79xZpt5Efi4GoWqInI03Lp/ZftTP8xPxVT9qqZqpn4lmf9OvnzeHibz9rPh5znVd0/StV1WrBw6civu3p2se0U0VUVTPX4GTHrHcdxNU2qo6iquZDYEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABmf8AWY4Iw8jaG2PJTbOFRia3oGdb0fWcvHmaLt7Fu/OLdqmPju1dpmmKo6q/XiJmYpp9dMEU5V4z2tzJx1uDi/eti9d0XcmFXg5X4Fz0u0RPzTct1TExFdFUU10zMTHtTHcTHcSFZ+EHNmm88eMux93WdZu6hq+DpePo2v15FyKsiNTxrdNu/Xd6/m5MRej+9N2mV7sPtyaP5NfSb5nv6pte9a1fZG5L9VrDv5dHvg6zjW6vaLd6iiqKrGTRTV/Ex95mn2p7hshxDyxsvm/jvReTdgataz9H1rHi7bqpn81m5Hxcs3I+9NyiqJpqif5j+3QJiAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAACuufeCNheR/GOqcW8h4l25p+oRFyzk49fpkYWTT828i1V9orpn56mJpqjumqJiZhk347cv7++l75G6/wAM824eXlbH1u9T/VXcP89EU+004+rY9Hz7RNEdV2/iv1mO+6rdNM7Uqu8gPGriDya2ra2py1tmNQt4dVdzT82xdmzmYFyuIiquzdj9vfrT3TMTTV60+1M9QCT8c8p8c8vbet7r4y3ppO5NKu9R/Uafk03Pw6v+W5T+63V/01xFUf2Spjtv76XXlp47a/kb98WuS8jXbWPM1Wf8Lz69J1mm1E+3pXR7Rav0xERExFz88/6cd9PpsD6rnlHwTqtOxvJ/iqvX72L1RcqzsSvRNXpp+3tV+n+FciPjr9Kmav5rnvuA2FHH/Bn1SfGPm/cuj7HtX9w7X3HruVawMHC1jT4m3kZVyqKaLVF6xVcoj2qmIia/TuZiPvLsAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAB4u69k7M35pk6LvnaOi7i06qZmcTVsC1l2Z7+P2Xaaqf/j2gFEaJ4L+Je2t96VyVt7hHQ9M3BomTRmYGRiXL9q1Yv0Ve1FyMem5FmaqZ6mJmiepiJjrqF7gAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAD//Z</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2022_9_21_10:38</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2021_9_20_10:40</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2020_9_20_10:54</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ך</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>ך</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>ך</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>כן, משתעל\ת בשל מצב כרוני כגון אסתמה או אלרגיה אחרת.</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>לא</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>לא</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wBDAAMCAgICAgMCAgIDAwMDBAYEBAQEBAgGBgUGCQgKCgkICQkKDA8MCgsOCwkJDRENDg8QEBEQCgwSExIQEw8QEBD/2wBDAQMDAwQDBAgEBAgQCwkLEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBD/wAARCAEzATMDASIAAhEBAxEB/8QAHQABAQADAAMBAQAAAAAAAAAAAAgGBwkDBAUCAf/EAEcQAAEDAwMDAgQDBgIGCAcBAAECAwQABQYHCBESITEJExQiQVEjMmEVQlJicYEWFxgkM3ORoSVDRFNjcoKSGSg0VIOTovD/xAAUAQEAAAAAAAAAAAAAAAAAAAAA/8QAFBEBAAAAAAAAAAAAAAAAAAAAAP/aAAwDAQACEQMRAD8A6p0pSgUpSgUpSgUpSgUpSgUpSgUpSgVjmoGouDaVYpNzfUXKbfj9jt6Ct+ZNdCEDsSEJH5lrPBCUJBUo9kgntWR1F2UafWDdfvtyHF9SreL3gWhOP20IsUklUKVfbkkyEvPN+HQmOkJKDyOUJ57FQUGB23eZvk3MyrrP2hbfrFEwZmc7DhZRk7vQqQ2lRSHUJcdbQVeCUIQ90flJJr3/APQ49QLVtHua574Xcejvnqdt2Gxltp6Po2VMiIP0PIWO3lXmr2t9ut9ogsWu1QY8KHFbSyxHjtJbaaQkcBKUpACQB2AA4r2KCIMQ9IbazaZBuWezszzy4PK9yS7dryplDqv6Rg25x/VxR/WqAwvaDtd0+Sj/AApoJhMZ1vjokv2hqVITx9nngtz/APqtv0oPDDhQ7fGRDgRGY0dsEIaZbCEJ5PPZI7DuTXmpSgUpSgV6c6z2m6FCrna4kstghBfYS508+eOoHivcpQYvJ0t0ymuuPzNOsYfcdPK1u2iOpS/6ko71D+4rYtqxpjqx/pRbDZ0Ow5GEqVd8SR7bEaaDx7gYQoBlSHOAVsL6R1DrQoL6QOhFKCQdm2/B/XvK7rolrFgbuA6r4+0VyLW4lxtmclAHuqaQ787S08hRaUVfIQpKlAK6a+rnn6i1liaJ7hNBN4NiiogvQslax7JZTSOkyYqxykKI45UY3xzfJ5JT0jwkCuhlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlArX2r2v+jOgtoTetXNRLRjbLiFLYZkulUmQB59mOgKdd4/kSa0Luf33RcCyQaD7dMbc1K1juKjHbtsBPvRLQo8grlLT2K09iW+QEgEuKbAAV8bQX067Am6O6ybv57erGqN5WJMtNzUZFrt3flLLbKgEPdI7fOn2wAEoQkDqUGstS/WgwC3N3JvR/RzIcnbYIjR7rc3hBiF9YPtkoSlxwp5BIQShSgkj5fI1Tte30wdoi7/ZNzm3zUKz5jnV4kZBf8kkRfbm3J1xRLYMSUhlSGW0r4AS4sArWoAdfTW7sFhWbefvJTNxu2xGNCtuzwbtEaFHSzCuuRcjhxKEgJUhCklQI7dLLR44eNXXmWA4LqLaRYdQMMseTW0LDoh3i3szGQsAgKCHUqSFcE9+Oe9BpnSrf5tJ1ilR7XimsVqi3SSQlFvvKHLa8Vnw2kyEpQ4r9G1KqhKjHXX0ptr2qdmluYLjp06yRSVKjT7Otaohc4+VLsNai2W+fIa9tX83A4qeduG7PVrYrn6drO9BiccWaV7dgyUhchERjkBCm3OOqRCP07Fxo/KUgDoQHVSleGFMiXGGxcIElqRFlNJeZeaUFIcbUAUqSR2IIIII+9eagUpSgUpSgUpSgUpSg0VvR20t7q9C7jpkxef2XdWJLd2s8lY5ZE1lK0oQ6B39tSXFpJHdPUFAHjpOrtiW7zKNTpd426bgoK7LrJgQLE5uQEoN3YbISp9IT8vup5SVhPyqStLiOUlQRY1Qf6kOiGV49Ix/e1oUx8Hn2mbqH7wY6O8+1J55W6kf7T2gVJWD+ZhxwE8NpFBeFK1pt114xDclpJZNWMNX0R7k2W5kJSwp2BMRwHo7nH1SrweB1JUhQHChWy6BSlKBSlKBSlKBSlKBSlKBSlKBSlKBSlKBSlKBXP/cFue1Z3Mapy9o2yqd7BiKLWZ560tQYtjIV0uNsOp/LwepJWnla1Dpb4AK6+zvQ3KZ7nmcs7JNqTipef38BrKL2wpQZx2ArgOBTiQehfSsFxwd20qCUguLARRG1zbPge1jS2Fp3hjIflK4kXm7ONhL9zmEcKdX9kj8qEc8JSAO5KlKD5+1zaNpXtVxRVpwuCZ1/uCEm9ZFMSFTbi55PKv3GurkpbT2Hk9SuVHXHqO7hLrpNo/H0y08MmTqRqrI/w7j0WGOZCUOKSh95PHhXDiWkEHn3HkkflVxWEuXFgRXp8+S1GjRm1PPPPLCENoSOVKUo9gAASSewArnrtZjv71d4+X7xb5HdVgunTpxnAWHknoddSlXMjg+FBDiniCOUrlN8E+3QVltR2/WbbNoZjuldsDLs2K18XeZjaePjbk6AX3efJHICEc9w222PpW3qUoFan3M7ccF3P6V3PTfNIjKHnW1O2i6BlK37XNA/DfbJ78cgBaQR1oKkkjnkbYpQc4vTx3DZnpDnty2D7j3Vwsixp9cfE5klZ6H2QOoQ0rUAVIUgh2Oo+UKKBxw2iujtRf6juz2drnh0TWHShhcTVTAUiZb3oYKJFyitK9z4dK0/N7zagXGT/F1JHHucpyzYBvDt+6zSlCL/ACGWNQcXbbiZFDACDI7cNzW0jgdDvB6gAAhwKTwB0FQVJSlKBSlKBSlKBSlKBXjfYYlMORpLKHWXUFDja0hSVpI4IIPYgj6V5KUHMmDG/wDhpb2WbYwtUbQrW5wJaC1fgWWaF8AcnwGHHAOT/wBnkDkrU1zXTUEKAUkggjkEfWtI7yduVr3QaDX7Tl1llN7aQbjj0pzgfD3JpJLXzH8qVgqaWfohxR8gVrD00NxN11j0Sd0/z5+QjP8AS+QMfvTEwFMlbCSpMZ5wHv18IWyvn5ithSld1Cgr6lKUClKUClKUClKUClKUClKUClKUClKUCps3ya7ZppNp/ZcG0giGXqdqhcxjeLNp45jrUB78vueAGkqTwo9kqcQpXKQqqTqPLc4zrN6jt7vktaDj+3jEWoTanCAhF6uqVLW6Ce3AihaD9lNg0GzNpm0zCtreFrgwnBe8yvX+sZLk8hBMq5SVHqUOpRKktBRJSnnueVK5USa3vU3ap+ojtC0kkO2696vW+73JnkKhY+2u5r6h5SXGQWUKHjha0nn+hrQN99Y/CJVvuV20s27ag5TBtSSuVMllqFHYQAPndcaEgNp5PlXHbg/pQZ/6nGtWQYzplZtvOmanX891lmCwxGIyvxW4ClJRIVwOSA6VoZHI7pW6QeUGqH256KWLbzovi+klh6FoscMJlyUjj4uYslch89ufndUsgHwnpT4ArlzpXju8nf7r1ct3Onc3H8BiWlz9g2e5XJYlt2htLQCmYbamll10IeUpTqkIT1vrKSggBFQq9OnXu8hNzy31DdWJF5Sr3W3YLkmPHjrPHPttCWeB2HdPRzxzwPFBd1KhE7It7uPApxH1FcnmoCR7abxanXFDjsApa5LxPbyrjufIrxotnq16LELiXrTrW+1tJADEhLcKcEADn5uI3KvPBK3SfsT2oLypUJW71QncAlos+6vbJqFphJUsNC4IiKmQHFfxBS0tK6fP+z93x5NVJpDuQ0M16iGTpLqbZMhcS37rkRl4tzGUdvmcjOBLyB3A5UgDmg2TXMTeto/mOzLXa2779vlr/wChpk3281tDQIY631AOqWEj5WJB/Mr9x/oUO6kgdO6+TleK4/nGM3TDsrtTFys16iOwZ0R4coeZcSUqSf7HyO48jvQfE0h1Ww7W/Tixao4FcBLs1+jCQyTwFsrBKXGXB+642sKQofQpPHI4NZjXMfbddr76em7q47T87uz7+mGpMhM/DrnKX+GxKcPQ11HjgLWUiO6O3zpZXwlKuT04oFKUoFKUoFKUoFKUoFc7dXoQ2feo7hmtFtR8Jg2uiFWDIkpJSy1clKQguq/dTy4YjxUe55k+OSa6JVNfqG6HL122tZVZ7ZHLl/xpAyayFA+f4mIlSloTx3KnGS82kdvmWk/SgpSlab2f6zo1+24YPqY9JD1ym21MW7Hq5ULhHJZkEj6dTjalgfwrT555O5KBSlKBSlKBSlKBSlKBSlKBSlKBXxsvzLE8Ax2Zlub5HbrFZre2XJM6fISyy0n9VKIHJ8AeSeAOTXpal6jYlpHgd71Jzu5iBYsfiKlzH+kqUEggJSlI7qWpRSlKR5UoD61yTgW7X/1c9aJFymzZWH6OYrK6EIB62YaDx+GgdhInOI+ZSj8rYV9ElCVhv3WD1a4F3vrenGzzTO56i5NMcLMedKgPiMtXfuzFRxIeH15V7QA79xWgNDtne4revm2p2V6z6syMKhpyr9nZfaoLRUuZc47KCWvYbUmOPabWhCVqU4Ukn5TySrqFoLtm0Y2144Md0nw6NblONpRMuTv40+cR36n3yOpXfv0jhCeflSkdq1j6fbCpGmWoGXraKFZfqnlV7UVBPKiqZ7PJ4Pn8Djv9vtxQefRz05tpWjLDLlv0wiZPdGgObnlATcnlKA/MG1pDCDz35Q2k8n+lRR6qm4e4ZrnVj2V6NNJMOFKiN3iJb2/bEu5vKSIsBITwkpR1oUUjsXFpB4LZrp5rPqbadGdKMs1TvYSqLjFqkXD2lK499xCD7TIP0LjhQgfqoVxp9M3ALzuI3qq1UzZxVy/w0uXmd1kPDkP3Fxzhjv8ARXvu+8P9waDsHt00Zs237RXE9JLL0LTYYCG5b6Rx8TMXyuQ99/ndUtQB8AgeBWx6UoFKUoPBNgwrlEdgXGGxKjPp6HWX2wttafspJ7Ef1qUtafTR286lzP8AFen8KVpTmkdYkQr5iR+FQ0+n8q1RUFLfY9+W/aWT+/VaUoIEte5TdFsqubGJby8ffz3TtToYg6m2GOpx2OknhCZzYA5PHHPUEufm4VINW7hGd4bqVjMLM8ByW336yXFHXGnQXg60sfUcjwoHsUngggggEcV9a4W633eBItV2gx5sKY0piRGkNJcaebUOFIWhQIUkgkEEcEGoyzHZtqHt4yG4aw7DshTZX31/FXrTe5uKcsl7SkElLHUeY7vkJHIA6uEraTylQbG33bWYm6TRSVZbWhDOZ42V3XF5nPSpMpKfmjlX0Q8EhJPgKDa+/RxX52D7j3txuglvuOSvqGbYss2LKI7qSh4S2hwl5aT3BdQAo9gOv3Ej8tZNto3U4LuQs0yNBjSsczbHlfD5NiN0SWrhaZKT0rBQoAra6wQHAB9AoJVykT9qJaGtl+9mya32sfB6Y68SE45lyAeli335RK40s+AkOK6lEnwFS1HykUF2UrVGuG6XQfbrbjM1X1Dt1qlKQVsWxtRkXCR25HRHb5c4PYdRAQCRyoVGb3qH7pdzF1kY7sj24yjbEOFhzJ8ibC0M+O6vnTFYWB36FOvEjnhNB0jr5OSZbiuG283bL8mtVjgg8GTcprcZoH/zuED/AJ1CkHZFvj1bPx24vfBeLQzI7v2bDfcaZWk/uKLfwzQI7f8AVODkHufzHN8S9J/ajZbkm9Zizl+fTyFF13JL4tYdWr95QjpaJ4PPAJPnvyeDQbIu3qA7NLLJVFmbg8XcWhKlExFuykcA8HhbKFJJ+wB5Pkdqy/T3dLt01Xu6cf081nxO93VYBbgMXFCZLoI5+RpZC18c9+kHjweKxebsM2dT7Smyv7ecQTHT08LYiFl/t45fQoOnx3+bv9a0Drv6P+gubWpmTobLk6bX2KrqBL0i4wpIA7JWh50uNq5A4Whfbk8oUeOAvmlcjdNN1u6jYJq/b9Ht4j1zyLBpyUssXR1xc5bMdPypkwpJ4U82gqSHGl8rCeAAkhKVdZLFfLPk9kt+SY9cmLha7rFamwpcdYW1IYcSFtuIUPKVJIIP2NB71KUoIh2Rw1aH7ndwW1T3kos0e4x85xeKlJCWoUwJ99Kef3W/chtf+ZtR+tW9UUbklDR7f7oBrSwoNQM+jS9Orz0jgKUtQVD6j9y9IQefsxwfpVr0ClKUClKUClKUClKUClKUClK+Rl+TW7CsTveZXhfRAsNuk3OUr7MsNKcWf/ak0HObfBJyHeJvFw7ZBiGUyoGL2GOLxl78UBSWpHtl0lSTwFltgspRySA5KII5TXQfTLTLCNHsJtmnmndgj2ix2lr22I7KQOonupxZ8rcUeVKUe5JJqOvSx0sNzwzJt3mbtiXnGrd3uEj4taeDHgCUrrbQD+UOSELUfoUtsgDhPe7qBU1en+DG0LutneBEm1Z1lMKSn6B1N1fUQD9RwoVStTXtHSjHNSNxunBJ9y3amv5EkKPJS1doUeUP7Ffukf14+nACdvWh1uTjWlGNaFWqWUzcynftS6ISR2t8RQLaFj7LkFCkkf8A2yqy70fdFjp9tvlamXGMG7nqNcTLQSnhQt8UrZjpP17rMhY+6XEmox9VWRcdUN9kbTyxp+IuMO12TGYrQ7kvyVKfQjt37man9e9dn8Bwy0adYNj2AWBBTbcbtcW1ROQAS0w0ltJPHbkhPJ/Umg+9SlKBSlKBSlKBSlKCbNz20m0al3NjW/TPLU6a6uYw0ZFvyyOQ2y+htJPs3BP5XWCkdKlKCilHIIWgFB57agbv9cfUFi4vs6sllwiy3S6z/bv18XPR8FdHIyypDsb3U9bTfCA50tdbqyAE8J6kqr/1O9YrsxhGPbVtNJhcz3WS4x7QI7LnC2LYt0IcUsjuhLqylruOFN/EfwmthXj0/NB7vt3smgjVmRbX8cYD9qyeE0G7lFupSkuTw4D1KW4tKVLQT0lISkdPQgpCZtiGw/QbL4mQZTrxaLnluqOJZLNs2TWm9zC7CjTG18tuhsAGSh1tSXAt0rQvk8D5ea6UWiz2mwW2NZbFa4ltt8NsNR4kRhLLLKB4ShCQEpH6AVzI0Z1t1L28b0rVpxuNAayLJ4kfEL7eW0kRMkaSriy3sKIHU8CVQ3VK4+VxBIK0OcdQ6BSlKBSlKDRu8Pa9je63Ry4YDchHi32JzNx26uI5MGckduSO/tOD5HE9/lPVwVJSREfph7osk0szefsi15U/bZsCc/Fxv43sqJMSsl23FX8Kz1ONHwSVJBPW2K6nVzk9VnaXMvVpa3c6Utuwstw5LL9/MPlD0iIyU+1OQpPf3Y/CeVf90kHke0AQ6N0rRGyncZF3PbfrBqI840L9HBtWQsN8D2riyAFq4HgOJUh5I+iXQPINb3oIl9Wpa7Pt6xPO4qHBLxDUG0Xhl1oDrQUNyE+fIBKk+CO4T37VbVSF6rOLTcl2WZZKgvFJsM623VxsAfitpkoaUnk+OA91/f5OPrxVJ6UZizqJpdh+fxwQ1ktht93QCSSBIjod4PPfn5/r3oMqpSlApSlApSlApSlApSlAqbvUaydeJbK9Ubi1JWy5KtjFrSUKAUsS5TMdSe/kFDquf5eqqRqN/VMQq8aCYlp8nkjOdRbFjy0pPBKXC6555HHdkdz28ePIDf22jDG9PNvWm+Fojhly04vbWJCQkp5kfDoU8og9wVOFaiPua2VX5QhDaEttpCUpACUgcAD7Cv1QKmzaeBctVtyeUdPKpGpX7KLg54Ih22IgJ/qOvv8A1qk6j/b1mzGnWn27TUSWR7eM6q5ldlp457RoERwD9SQgdvuePPagjrQaxN7lfVuy7OJTInWjDr5cr0pbncKRbimFBWD9w6Iy0jzwj9DXYWua3op6drY0/wBRNZ7mlTs3Iry1ZmXne6y3Gb951QPnhbkpPP3LQ+1dKaBSlKBSlKBSlKBWK6pakYzo/p1kOp2YySxZ8bgOz5RTx1rCR8raASAVrUUoSOe6lJH1rKqgff7dbpuH1s0w2H4fcH2Wb9LRkubSGP8As1sZ6lIQT456UPOBKuB1iN/EKDy+n5pflesGaZBv91vjBWS5q49HxCC5ypFotIJb6mgocp5SktIPAJbC1kn3iavOvRsdktONWW345YYDUG2WqK1ChRWRwhhhpAQ22kfQJSkAfoK96gnTe7tJse63StdpjexAzawdc3GLsR0qZkcd461juGXelIV9iEL4JTwfY2TbhpOvekSI+XoXC1Fwd845mlsf4D7FxYJQXlJ7cB3oKvHAWHUAnoJqg65x7xrRqZtj3iYluX0GtJnOZ7bn4GQ4+gqDV9fhIDjjBA8PORU9bRAJ92KeAtS+hQdHKVg+i2suB6+acWnVDTm6fGWe7NkhKwEvRnk9nGHkAnocQrsRyR4IJSQTnFApSlAr158CDdYMm13OGzLhzGVx5Ed5AW260sFKkKSeykkEgg9iDXsUoOY+2uBI2I7/AHI9tt0fUzp9q2ymdirzrgKEO9TioiCo/vAiRFI/Mtfsq8EV04qQfU20FnaraCHUTDw+zm2lTysls8qKSmQlhvpVKQ2odwehtDo479cdAHmtw7TdcWNxe37D9V/w03C5wvYuzTaelLVwZUWpICf3UlxClJH8C00GpfVPzpvCdmGXxQ4lEnJ5MCxRuVcclx9LrgH3/BYe7f37gEVubazZEY5to0psiCkmJhlmQtSVchThhtFZB+xUSf71Ee/x+Tuh3laRbL7PIdcs9sfRe8pDLhT0BxJccCiPyrbhNrKD95QH1rpPChxLdDYt9vjNRosVpLLDLSAlDbaQAlKQOwAAAAH2oPNSlKBSlKBSlKBSlKBSlKBUfeoQhD+RbZYj6Q4w9rfjocaWOULHuKHBB7HsSP7mrBqSN2kI5vuq2saZe4r2EZJdcxkgFQCDa4zbzBPH3WVJH9e/Y0Fb0pSgVzJ1uy1zTvb3vhxJMlxqa5qGxJS34UWryi3pPcfuqaS5547Djnk102rj96sFxk6b6n5vjTMZYhaw2rGL246E/KqTa1y4ykk/xBssEn7FI/oFwemfiLeIbK9OmfbCX7qxLu76ungrMiU6tBP/AOL2xz+gqoa1btVtjFn2x6S22OjpSzhFk57EcqMJoqPfuOVEn+9bSoFKUoFKl/cB6jm2Db7Ik2S65c5lORxyULs2NoTLdaX37POlSWWiCACkr6xz+Q1pqBuv9RDcLw7t82r27B8ek8Bq+5k8vq9s+Hmw4WQsH+Rp4D7nzQdBax7JtRdPsKUhOZZ1j1hU5+QXO6MRSr+nuKHNRzC2M7p9VVImbnt7uVusud5Fkwb/AKOin9A6EoQrjtx1Rqy7GPSs2X2BRfuun10yaWpSlqlXm/S1rUo88lSWVtoUTyfKT37+aDetw3DaIwsRvecRtU8Wulqx+A/cpzlru8eWpLLSCtXSltZ6lcDgDySQB5qTfTMx+/ar5Dqjvfz6KtN41KvDttsiHVFZiWphY6m21Hy2FIZYHPcfBfr3m31MNse2/SO6ac6baA6YptmoOeXTpCGLrLeQI3UlhpHsvOrSlTr7qQlSQP8AYuduTzVA2T009ftLLNCgaF76c0x5mG2emzyWXlW4OKPUoobQ/wC2kFfJ7sknqP68h0HpUCLc9XTRMe+9/l3rba2B1LQ2lEaYWge4AAikr4+wd+n5jWR6YeqRphOyMaebjcFyHRbL0FKHGL8w4qESewJeKELaBIPdxtKAOPnPegtipw3+4/dJW3abqHjbHuZBpZdrfntq78dLlveC3iT9B8OqRz57fSqFtlztt6t0a72a4Rp8CY0l+NKjOpdZebUOUrQtJKVJIIIIPBr1sox625djN3xO8N+5AvUGRbpSO3zMvNqbWO/8qjQQrfLzbNmesVh3JYEpwbfNdVRXcnhtIAj2C5SW0rjXNtCR8jbiVcrA7f7Qf9ykX224282l1pxK0LSFJUk8hQPgg/UVHe0rGbRrTtCyPaxq3HMuXgU+56c3xBAS4kRnCYshrkdulpTJbX3HU1zyeK8OwfVnJsZm5Fso1nmOf490qWpq0y30lIvdh6v9Xfa57noSpscefbW15KVkBZlKUoFKUoPDLiRp8V6DMYQ9HkNqadbWOUrQocKSR9iCRXLLZNr3jmy7/SU0Z1MmOtWzTW7Sb3Z2HFdL07h74MNtJPfl4iAUngp/FKjwOTXVOuHm7RjRzXr1OWMUjXZxnHr1kFmxrILhFWOHpifbjPhpXhPBShkr7gKQpXceQrP0vNMMyz7Ks+3y6sRyL5qHJfiWRC0EBMQuhT7rYJPDfU20w39QlhfchQ56IV6NisdnxmywMcx+3MW+2WyM3EhxGEBDbDLaQlCEgeAAABXvUClKUClKUClKUClKUClKUCpc1Ljvp9QvReU+U/DOYTkrccKP/XJUyV8D79Kk/wBuaqOps3HpFn3M7Y8yJAS1kN/x9ZJ4BTPtS+E/164zZH6p45HNBSdKUoFSXvQxDFpOs23DOMzxaz3+xnMZOF3GDdYLUuM+LtFKY/uNuJIPQ/GbUgkdl8ffvWlTZ6htvkHa1kGXW5gO3HB7laMrhcnjpXDnsuLP/wCr3f8AjQUfGjR4cdqJEYbYYYQltpptIShCAOAlIHYAAcACvJXggzYtyhR7jBeD0aU0h9lwc8LQoApI5+4INQpvp9Q6dpVfk7ftt8RvI9Uri4mFIkMsfFotLrnyoZbaHIelkkEIIKUduoKJKAFK7id1GjG1/GTkGqOUNMS321Kt9milLtxuBHPZlnkHp5HBcUUtpJAKgSAYZGWb5fUpeXHwht3RnQ+W4tly4lShIucfkpV846XZRI6gUNltjylalEcnKtsfpjXG+X5Oue9y+Sc2zC4LTLFgmTFSmWVcAp+NcPPvqT+X2Un2kgcfOOw6Kx48eHHaiRGG2GGEJbaabSEoQgDgJSB2AAHAAoJy227Atu22qPGuFgxVrIMqaCS5kd7bTIlBweSwkjojDnnj2wFcHhSlVSNKUClKxvUnM4unOnWU6hT2y5Gxeyzry8gAnqRGYW6ocDv4QfFBzbxP/wCaL1f7xfHQJeP6QMOoZSohaEKt4DCQD45/aEhboA7/ACn7E11Irmz6MGGTLhiuqOvF9V8RcsrvzdsD6+OrllBkPqH1AWuWjn9Wh9q6TUCsJ1X0U0q1xx1WK6r4Laskt5CvbTLa/FjqI4K2XU8OMq/mQpJ/Ws2pQQLN2R7kdrs+RlOxXWh6RZS6uS/p5lzvvQXuSVFDDp4QFKPSkE+yvgfM+azbRn1HMKveUf5Sbk8SnaM6jMLQyuFfOUW+UpXZKmpCwAgKIPHucJII6XF81Yla31028aR7jsRcw7VjEo11jhK/g5gAbm29xXHLkd8DqbVylPIHyq6QFBSe1BpaxpGjnqGXi0NqS1YdfMTRd46Qr5VX20jodShPj5oi/cUR5PkHjmvU366J5W/EsO7DRBssaoaSKM5KWkcm8WccmTDcA7r4SpxQH1Sp5IBK0lMP6xSdYtiupemmnWpNzl5Rh2D5ZGybAcodSfdFqKgzcbWonnpBaWklAPyFtJSCl1PT2ZQtqQ0lxtSHGnEgpUCClSSPI+4IoMB0E1pxTcHpNj2rOHOj4K9xgt2OVhTkOSn5Xo7n8yFhSefqAFDsoGtg1Bui8RWzTe/f9vvCYmmWtjbmSYa0FBLFvurY/wBYiIT2CAQFJAH0TESO5NXlQKUr4Wc5tjWm+G3rPcxubdvslghO3CdJX36Gm0lR4HlSjxwlI7qJAAJIFBOvqGbrhtl0Zci4vJKs/wAzDlrxtlv5nGFEAOzOn/wgtPT2PLi2xwR1cc9txOz+btV2aaW6qTYiEakKzJm53yQ4nl2GqRGU6xFJ+qWTFQFck/iuOcEg9qM2kadZNva3F3HffrFapEbErJL+D06skn5kAR1qDbv2KWVdSiR2VJU4QQG+k7x9UzGU5Hsmzl9Lalv2V62XNkAc8FM1lCz/AGbccP8Aagqay3aLfrNAvkEkxrjFalsk/VDiApP/ACIr3a1htdyH/Fe2zSzIVOFxydhtnceUST+L8G2HBye54WFDmtn0ClKUClKUClKUClKUClKUCpp3zTFYvjmlWqK0I+DwbVKwXO5uKA/DgvF6E8eT4/8Aq0H+oFUtWmN5uCf5lbVtUcRSyHnn8bly4zZHPVIjJ+JZH9fcZRx+tBuela0206k/5v7f9P8AUlyR70m+4/Dfmr55/wBcDYRJHP14eS4Of0rZdArD9YcCa1T0nzLTV11LQyixTrQl1Xhpb7C20r/9KlBX9qzCtebh9SndHdCs81PiqZEzHLBNnQQ82VtqmJaUI6VpHcpU8WwfHYnuKDmzevUd1eu+junG2nb7iNyf1ik2lvHr/K+G9x+BKjFUVSI6D8peWln3lOq/DaSr78lultg+wCLtwZf1T1aciX/VW79a1SvcMhu0tufnQ04rut9fJ9x7z3KUnpKlLmr0iYcdrXHKsl1Qs6383z3GP8VY7d5pPuvwjcX2J60A9it19CFdQ79LauPlUrnrRQKUpQKUpQK0Zvlucu07QNXJUJSQ4vFZsZRUoge28j2l+CO/QtXH3P0Pg7zrU+7ZhmRtW1iQ+0lxKcCv7gSodupMB5ST/YgH+1Bpz0pcdj2PZLhk5lSC5fJt1uL/AE8HhYnPMDuCeT0MI/UeD4qu6jz0m2nW9lGKrckqcS7c7sttJ44aT8Y4OkcfTkFXf6qP6VYdApSlApSlBpbd/t+x7cjoPk2A3W2pfujcN6fj8hI/Fi3NptRYUk8E8KV8iwPzIWodjwRpb0tN0cvX3Q1eE5XIQvK9OBGtT7nUSqZbi3xEkK58r4bcbX57thRPK+BaVcY9Mbg9ss3a3zUVnoYxC0ah3LT7Lm218IjWecv4m2THeOTzwHF/0hdAPKuaC+fUR0evWo2hJz3BELbzvSqc1mOOyGUBTwXGIW+2n78tp6wkc9S2WxxW5tBtW7Nrto9ierViCER8ktrcpxlKur4aQPkfY5+pbdS4jn69PNZ0hbUhpLjakONOJBSoEFKkkeR9wRUX7OGndv8AuS1i2dukNY8l1Of4Q108Bu3SlJTIYQT3KGnFNIA+7bqvqaC065+eoPnV63Aap4V6f2ldwWZ2Rzo90zeWwErTbre2Q6htzv2KUJMhSDwT0xgCfc4rbu9nelC25WqHp/p7bv8AE+rmWBMfH7Ew0XywXFdCZL6E9yOrshvy4ocdkhSh62xTaNetC7TeNWNY7gb5rDqAfisguDziX1wW1q9z4RDo8kq4U6UnoUpKAnlLaVEKWw7EcewDFLRhGJ21u32axQmYEGM2OzTLaQlI/U8DuT3J5J7msR3I4kM82+ak4cGwty74pdIzAPPZ5UVz2ldvsvpP9q2PX4eabfaWw8gLbcSULSR2UCOCDQSl6XGVHKNlGCtuuBb9lcuNqdIPj25jqmx+nDS2/wD/AHYVhUE+jfJ+H295ti5eW6LJn85ppSkgfhKiROPH16krP96vagUpSgUpSgUpSgUpSgUpSgV432GZLDkaQ2lxp1BQtChyFJI4II+xFeSlBHPpm3J7HtONQdvtweWZmkOeXawtIWrqIgreU4ysfopz4njz45579rGqHcSf/wAkPVLy7Fn1+xZtdcSj3qEgdkLucNKkqTzxx1dLExZHn8UfcCrioFS36nECbcNkOpLcK4Iie01bn3uogB1tFwjKU3ySOCeBx9T+Xg9VVJUpeqRdP2Zsd1ESlRS5NVaYqCP5rnGKh/7UqoNJ6ly4Wk2kW0DeLjUNMW24VbLLYsjTGSOP2HcoLSHVLCRwQ2sL4HAPuPDtz46LMvNSGkPsOocacSFoWhQKVJI5BBHkEVP2L6NWLVvYjiuil3ITCvmm1otqHlAEsvCAyWX/ABwVIdShzx5T4rFfTm1hu+c6LP6TZ71sZ7o9MViN+ivE+77bBUiM6ee5BQ2W+T3KmFn6igq6lKUClKUCsZ1OxJGfabZZgrqQpGR2OfaVA8cESI62jzz2/frJqUEM+jtlKr5tLfx57lL2L5TcLd7agAoIcQzJB488dUhY79+UkfSrmrnH6VFwTherO47QeWtSXsfylUmM2VlRUGpMmK+fJHb24/ceeryeBXRygUpSgUpSgVBWR6PY7qvu53P7fsnX7MXVXBcdyKK8UhXwkiEgRWpKE9uSh4oWe/fggnhXa9ajjV2/2jTr1IdMcxvV2jWm33/TS92i4TZkhLEdEeI65N5WtZCQEn5j447H6UHn9OPWHJr3p9eduerCixqNozMOPz2HVcrkW9BKYryT++lISWuoc8pQ0sk+5ydKepHuKwnQ/cBphqtplk1nueqmFNXC2Xax9SnEKt0phQbTLWjsjoWtSg0VBZ93qAA4VWhd1e5ZvOdz0zWPaHfb5ikF+DFwPLdQExlNW59Uh0Jbe6whS2gltsAOfK4RGSUJHSFKsyP6amk+B7adRMKt0ZeV6h5XYJXxOVXVsOSn7ilJea9rnqLDZkIQopBKldutayAQH0NkG0PIsLulw3ObjnzfdaM0UuW65JUlwWRh1I/AbA+VLpT8qij5UIAaRwkK67JrQ+xfU97V7adpvmM2X8TPTaE2uc4fzqkQ1qjLUv8AmV7PWfv18+DW+KBSlelepq7bZp9xbSFLixXX0g/UpQSB/wAqCG/R6hNf5DZ/fW/mRc9RbiWXAeUuMpixOlSf05Uv/hV41GHpG2hNt2Y2WalKQbtfLrMUQCCSHvZ7/c8Mj/lVn0ClKUClKUClKUClKUClKUClKUEPep9ZbthNm0w3ZYnFW5d9IcqjvTPb+Uu22StCXELP1SXG2m+D9H1/fvZ+NZFaMvxy1ZZj8tMq13qExcYT6fDsd5sONrH6FKgf718LV7Tez6waXZTpffgBCye1SLctwp6iypxBCHQP4kL6Vj9Uipc9LfUu83PRy+bf84Cmcw0YvL+PTmFn5hFLrhZP0JCVofaHb8rSPvQWlUx+pXjrmTbJdTYjDIW9EiQrigkclAjzo7qyPt+GhY/oTVOVrfcpj4yvbvqfjfsLdXcsPvEdtCEFai4qG6EdKR3KgrggfcCg+Ns8yQZbtV0mvfWFrXiFrjuqH7zrMdDLh8Dj521dgOB9OR3qat29iv20XcPYt9On9vfexK8qYx/VC2REfnjrUlDc7p8FXZA5+X8Rtoc/jLNZ96VmWR8n2UYZDQ+HZGPyrnaZPfkoWJjryEn7cNPtf24qossxTHc6xm6YbltpYudmvUVyFOiPp5Q8ytJSpJ+3Y9iO4PBHBFB5MaySxZjj1tyvF7oxcrReIrU6DMYV1NvsOJCkLSfsUkGvpVz/ANtuW5Dsc13Vsr1Yur8rT/K5Ds/S7IZSvlR7jnKre4rskKK1ccDjh5QIT0vp6egFApSlApSlByi1lyaTsT9TlOr9zZdZwHVSOF3J5KeUhh/20TFdh3UzKaRIIA6uhSR3KuT1XiS4s+KzPgSWpMaS2l5l5lYWhxChylSVDsQQQQR2INTxvy2wxd0Wgd0xi3xkHLLF1XfGnuB1GWhB5jlR8IeRy2e4AUW1HnoAqTPTt9RPCcWwuz7bdxF2mY/esfeXa7TermnoiCMk8NxJS1EKYcaPLaSsdHQlIKkkdw6gUrEEaxaRuXONZW9U8QVcJqgmNETfIpeeJPACEdfUok9uwr7WQ5Xi2IxE3DK8ktVliqPSl+4zG4zZP2CnCBzQfVpU5ajb/NteDyW7DjeZHUbKZayzBx3B2/2zMlO8fkCmSWkn7hSwfPY8EVg7+nu9TdOz8RqXmyNAsBmg8YxjLglZHKYUCCmXOICGFEHw0PB6Vo5HNBn+4TfNoht/mjE5Nxk5fnUhYYiYljaBMuC31fkQ6E9meSR2V85B5ShXioH1FwrXPd1u90WsG83FG8CxjMUXc2LHrdIbbmxIcaMqQUPLUFLDjzjbKD19KvzdKGjwK6Q6G7UNBtu0RKdMsBhRbmpHTIvcv/WrnJUR8ylyXOVjq5JKUdKO54SKlrd/lFuk+pBtexAB34q1+9cHlJSFDplOrbbHAPI7xVkkjgAg9+DwFD6v7VtPb1tOyzblpth9uslskWd79jw46OEIuDfD0d1aySpay+22VLUSpXfknmvNse1Uf1i2saf5fcXi5dWbYLRdOv8A2nxkNRjOKWPopftBzj+ceK3rUdbaLk3t13Gao7a8zYXZrfnmSy8507eeUPhbkzIQgzIkdfhK2VJR+Cfm4C1cccKUH49OHjE2ddNEiT04HqjdUQ0k/lgyCPY4H0B9lxX/AKqsior0KlQMb9THcBhuNTGXLff8Zs9/urKOSWLi0GUBPPPAJTKWsj7uDxxVqUCtJb09Xk6HbYc/z9pwJntWtVvtoPkzJREdkgfXpU4FkfZBrda1obQpxxQSlIJUongAfc1zYv2oN59TPchZdOMCt8ljQTS27tXnIbo8khN9ltKIbbHB46HPmQ2jnq9tTrquD0ISFfbL9I5Ohu1/T7Ti4KWbhCtfxk8LHBRLluLlPN+B2Qt5SB254QOa3XSlApSlApSlApSlApSlApSlApSlArn7qsXNpnqPYfq1GQYuD69RU45fykfht3YFDaHCPCOV/CLKjx2VJP3NdAqm/wBQTQZzX/bHkthtEJT+R4+kZFYQ2PxDLjJUVNo+vU40XWwOR8y0n6UFIUrQ2yHcA3uS244vn8uSly+xmjaL+kEdSbjHAS4sgePcSUPAfQOit80HPP07Hxoxuc3EbTX1ezDt95OS2COfl6YpWEE8fUqYet/j+E/26GVzg32KuW1beNpVvTtMR045d+nGsu9hvnqSlKkqKv4lriqJQP4oSa6K2y52+9W2JeLTMalwZ7DcmNIZUFIeaWkKQtJHkFJBB+xoNR7r9tGLbpNJ5mB3laYF5iqM7HbykH3bZcEg+24CO5QfyrSPKT24UEqGs9jW5vJM/g3bb7ryf2XrPpuv9n3eLLWA9do6OyJrfP8AtOU9PWpPIV1IcHyupqsqmrddspxfcJIi6i4hfJWDas2FCFWPK7c6tpwKb5Lbb/QQVI5UQFp+dPPYkAoIUrSoy2z718hZzZ7bJvDhRsM1YtRSzEuDxSzb8ja8IdZX2bS4vgkBPCFn8nSrlsWbQKUpQK0BuS2N7fN0fRcNQMaegZA0AhGQWVaItwKAOAhxZQpDyR24DiFdP7pTyed/0oOebXon7ckxHEPam6jrklQ9txMmClCU8jkFHwxJPHPfqHnx275Fivo7bW7PIbk5Xfc7y32uhDbFwuzbLKW0/uAR2kLAPcdl9h44Pc3VSgwLS3QbRnROD8BpTppYMaSpsNuPQoaRJeSPAdfPLrv/AK1Gs9pSg8ciRHhx3Zct9thhhCnHXXFBKEIA5KlE9gABySa5M7dNQH95/qnPayW+CtOL4Pb5rttCioj4BhpcSKtRPHStx2V7/QPBKh8wSVGs/VD1rf0d2n36JaZxjXrN328ZhKSohaW3gpUpQ47gfDtuo5+inE/oDIGwLcftY2YbfrhlufZj+09QM4lqlyLJZIxmTWIUcrbjMLUCGWlEl13hbiTw8kEcpPAddq59+qprdhenZ0elQr5bpOW4fn8DJXbdElI/abMBltwuDgHltt09CfmHCiB9Aa0nlu/jenvKu0rAdoWl9zxmzOLMd+5QgHZqEK4HL09YSxD5BB+TpWn6OGtDWXZlcHd5mCbd8zzmLmmS3GW3ds9ct7zjzEBlJL78VUhfC3Hyw2StZCQFPtpHJBJC2fSxxLK88zXWHeFmNtkwDqNd3WLOy4ohJYU+qQ8QD+ZCSqO2hX/hrArohXggQYVrgx7ZbYjMWJEaQxHYZQENtNoASlCUjsEgAAAeAK1tuS3A4Ztm0lu+qmaOhxuEn2LfAS4EO3KcsH2ozfP1UQSogHpQlayCEmgnn1N9yVw0601iaA6a+7O1H1XIs8OJDPVJjwXVBpxaUgE9bxV7DY7ElbigeW63jtD2+wNs2gmN6Wslp25sNGde5LfiTcnuFPKB+qU/K2k/wNI571LuwjbvnGqWe3DfnuYjGRlmUuKfxS2yGulFuhlPS3JS2ruge3whgHuGx7hKitKh0HoFKUoFKUoFKUoFKUoFKUoFKUoFKUoFKUoObGB3aN6f+/fINNchf/ZmkmuKhdLHKd+SJbrgpw9KCr8raUOrcYP2Q5GWshI5HSetLbsdrmE7sNLJOn+UrMG4RlmXZLw22Fu26YBwF8duttQ+VaOR1J8EKCVJlraru5z3QDOkbON7L/7LvdtCWMZy6ZI6otxjE8ModfUAFJIHDbyjz2KHOlae4WHuP0SsW4fRbKNJr6hpP7ZhLEGS4DxEnIHVHf7d/kcCSQPKepPgmpo9KDVi+ZDovfdDc7lOpyvSW8u2Z2HII95iCSfabV9T7bqJDX8qW0DxxVxVzn3b45l+ynczB31aaWh2fheTFu06iWmPwO7ikI94DsE+4UNKSr6Po+Y8PEUHRilfFwvMsa1DxK0Zzh12ZudkvkRudBltH5XWlp5B4PcH6FJ4IIIIBBFfaoNVbgNsWjO5rG0Y5qzibU9UUKMC5MK9mfAUryWXh3APAJQepCiB1JPAqc4uyrd3pGlMXbtvivX7HYHREsuZ2xFxbjtgdkB5fuJA/RDKOPpVw0oIm/bXqz6fuIbl4dozqfGQPnVAluQJLoH2U8uO2lR/8hHb+9e61v8AdTcJ/C152P6uYz0H23JuPxkXyH1ff3UhpAHk8BSjwO3VVmUoI9b9UzbY+hCY9h1JdlOBITERijxeKz+5x1dJUPHY8duxNfp31LcDDXxULbTuInRCOoSo+Do9pQ5I7FUgfarApQRS76q2lLCVLf286/NpR+YrxKMAn+vMvtXpy/VKs81xUfDNpuuV4eABS27j6WSfvyG1ukVcVKCEjvC3+58C3pZsBnWXrJDT2XXRTA7fvKbeEUjsfHV/c0ON+r3qEC5Lz7STTNpwkqahxhKdQD+6nralDt4/2nP6+DV21+XHG2W1OuuJQhCSpSlHgJA8kn6Cg4Nbn9JtbMl3X4ptqz3X27ao5XOfgxpD7vu/C2d+a4FKbaaUtQSlMctPLUEoHCuOnhHUemuI+nJsd0Yty8lventuuLdsb92TdcvuSpLCEAd1utuqTFA+pJbA71HOqepm2faru6zTc3Z9V0azZvdHJj1mxq3xkCJZZcge2pUi5pWttSWmvcaS22guAK4V08dR9qzbft9PqP3eLmW4HJH9OtNC4mRDthjLYQtvuQYtvKupZ4PaRJVzwvlBWB00Gf7jPUZauEuFtp9P+wIvF+uijbmrvabeER43IVy3b2uEpUoAFRfIDSEgqHUPnTvfYdscZ2xWu4agah3ROQ6q5W2o3e5F1TyYbS1hxcdtxXzOKUsBbrp7rUBx2TyrZ23fZ9oNtht/taY4e2m7us+xLv08iRcpKe3IU8QOhJIBKGwhBIB6eQK+nuG3PaP7YsSVlOqWSIjOPIV+z7VH4cn3FY/cZa5BI54BWohCeR1KHIoM01D1Dw7SnDLrqBn19j2iw2ZgyJct89kjwEpA7qWokJSkclSiAASa52aW4dmvqea4ta9atWiVa9BsJlus4pj8g9Jur6VJCuvjstJUgF5YJHypZSTwtSf5juku4b1NMxtepev8abp/oZa5HxdkxZlxSJN1HHAXyQFHqBIMhQHylSWUjqKx0lxvG7Bh1gt+K4taItrtFpjoiQoUVsIaYZQOEoSkeAAKD6DbbbLaWmm0oQhISlKRwEgeAB9BX6pSgUpSgUpSgUpSgUpSgUpSgUpSgUpSgUpSgVqbcXtf0g3RYknFdU8fMhcTrVbbpFX7U23OKHBWy5wex4HKFBSFdI5SeBxtmlBBGCXzeVsZQrAM50+vmvWlEI9Flv8AjSS9fLZGSAEsuxSSpaEpHZJPSjvw6UgITsi2b7NlmvFuuWk+c5YmwrvkRyDcbFmkB21FTTielTa3XB7KVd+3DvVzwU9xzVX1hupejelWsdoNj1S0/seTROkpbFwhoccZ58lpzjraP6oUD+tBAemmY5F6Y+q7WlGf3eXf9ueezFSsUylXD37FkOd1IdUgcceC4EjhQHvNgEuorpPBnQrnCj3K2zGJcSW0h+PIYcDjbzagClaFDkKSQQQR2INQlqd6UmMTcbumOaE605ZhFnufKnsXubpu9iWrnlJSy6oLQsHuHSpxaT3HetQYBhfqQ+nlj9w/ZePWLVbTO39cqRboc5yT8C0DypyOhQRJZ7clQSh1sfOop8roOqdK53aX+rDmupNsfuVo2YZtfWYBCJ7uKXBV3Mc9PIU42iMlTIPSvjrPHA8ms5R6sGhVqX7OoelureFOoIS4q8Y2hLaTyR5S8Vdu3PKB3PHegtilRVcvVz2kMOqj2BWb5K8EqUlq1Y+rrVwOeweW3/TvwPvwO9fNk+q/gryeuwbaNbZyFJ5bU5YWWwtRHYfI8vsfuOf6UFz0qEXd8+8DUZSbdoXsIyyO8/yGrlmDrkKJyOx5DiGUEA8jn3x4+/j1V7WN/e4kKf3H7nmMAsb46v8ADWCtlKgO34brqCgEc9/mcfHb/gFuZVnWEYLCNyzfMbHj0QDkv3W4MxG+Pv1OqSKmvUb1Otp+DykWbHMruWoV8eX7TNsxC3qmrdWeyQl1RQyrk/wLUe3jxz8XFfSc2j2ab+1Mtt2WZ1OWoOOyMgvzpU4sfVXwwZ6vHhXPbseapTTnRPSHSGIYemGmmN4whQ4cXbbc0y67/vHAOtw/qok8cCglBeuPqQa8hJ0Y272HSSxPnhu755KUuYR9FfD9IW2OO/BjrH2Uax66enHuK1zfS/ut3mX29QFudb1ix6KWYZ+pKAooZQfoD8Me3/Cug1eORIjxI7suW+2ywyhTjrriglCEAclSiewAA5JNBPeh2wPa3oC/HuuI6cR7nfYxSpu935fx8xCx4W31j22V/wAzSEGt/wByuVus8CRdbvPjQYURtT0iTJdS00y2kcqWtaiAlIHckngVJmsHqV6MYfeTgOi1quus2dPn24tpxNsyIxd+gXKQlQUP9yl0jweK1ijaxu93p3Ri+7zM1/y+wBtxL8XT/GX0+49weUmQsKWgHjg9TinVglQCGeaD7up/qH5JqZlj+iuw7An9RMr6i1LyZ9gps1sTyUl0KUUhYBCuHHChokJ6fe6uK+1oL6d8aHmQ123b5edWNTZRQ+UTB7lqtzgA6Q22oAPFHHCeUpbT26WwQFVUWlej+meiOKM4TpXhtux2zsq6yzEQep5zjguOuKJW6sgAda1KVwAOeAKzGgUpSgUpSgUpSgUpSgUpSgUpSgUpSgUpSgUpSgUpSgUpSgUpSgUpSgkfXXYcxeM2XrxtezVzSbVVrqcckwm+LXd1HupEuOAUjrIHUoJUlXBK21q7jF4e9/XXQxlVg3obZMjisRUlt3MsMji42eSgcAOOo6uGQRyogudX/hJ8C4KUGmdFd1e2DWNpq3aRao41Jkuq5RaefgJhUfPTFeShxXfyUpI/XuK3NWitXdj+1rW5TkrONILKm5OHqVc7Ug26YpX8S3I5QXT/ALzqFaek+mm7iqlOaEbt9ZdP+e6Yv7ZVNhp+w9lJZKk/opSu/wBaC1qVDL2gfqk4ofhcK3l4ZkURB4QMjsDbDihwBypSYj6+e3jrI5/rXiVo36td64jXfdbpjZWCela7VaEPOKSeO/4lvSQRx26VDyeTQXXWLZvqpplppFEzUXUPG8YZUCpK7vdWIgWP5fcUOo+Ow58io+/0CN0+YIUdU/UKz51t7kPQrBGdhNKB57FSZCUkd/Ba47D9OMt079LLadhzqbrlmO3jUG9qIcfuGTXNx73XePmUWWihtQJ8BaVkD6nzQeLUH1NNF403/B+3+xZBrTmsgFMW04zAf9jq456nJCmz8gHcqaQ5x9eO5GKWvZ5r/uwuCM23159KtFk5C7dppik32IUZPPI+LdSVBxfn8qlr7jh1IHQLNwzT7A9ObZ+xdP8AC7FjUAkExrRb2ojSiPBKW0gE/qe9ZBQYPpVohpHohZjYdJ9PrNjMRYSHTCjgPSOBwC88rlx0/qtSj+tZxSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlApSlB/9k=</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2020_9_20_11:11</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>שדגכ</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>כן</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>לא</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>כן</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wBDAAMCAgICAgMCAgIDAwMDBAYEBAQEBAgGBgUGCQgKCgkICQkKDA8MCgsOCwkJDRENDg8QEBEQCgwSExIQEw8QEBD/2wBDAQMDAwQDBAgEBAgQCwkLEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBD/wAARCAEzATMDASIAAhEBAxEB/8QAHAABAAMBAQEBAQAAAAAAAAAAAAcICQYCBQQB/8QAQRAAAQMDAwIEAwUEBQ0AAAAAAAECAwQFEQYHCBIhCRMxQSJRYRQyQnGBFiNDkRUzUmKCFxgZNVNVY3KSlaLB1P/EABQBAQAAAAAAAAAAAAAAAAAAAAD/xAAUEQEAAAAAAAAAAAAAAAAAAAAA/9oADAMBAAIRAxEAPwDVMAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAB8666k07Ykc6+X63W5Gs8xy1dUyHDM46l6lTtlF7/Q+RFuntjPI2GDcbS8kj1w1jLvTqrl+SIj+4HUA/MlytzqL+km19MtJjq+0JK3y8ZxnqzjGTh7xyH2A08qtv8Avnt9bFaqIqVmpqKHCqmUT45E9UAkEEH33m/xD07HNLcORehJWwN6npQXeOtVUxn4Up1er1+jcrnt6kaan8VjhRp5HJR7kXG/StTKx2yw1i+2cI6aONi/o73/ADAt2Civ+mS4j/7t3A/7NB/9B2Nh8VfhJesNq9z6+zvcuEbX6frvXOPvRRPanz7qgFuQQlofmxxQ3Gu8Ng0lvtpapuFQ3qhp6ipWjfKucdLPPRnU/wDuJl2O+ME2IqORHNVFRUyip7gf0AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABnpyB50cta3evU/Hfi/xxrJ7vp2oWnnvFxpJKp74lRvTVMj+CCnicq/A+V72uarVw1V6Uq7u5wz8UzkRdaa+bx2aovM0b1jhpqnU1qjpqJqqmXMp4JkhYi9sqxvUvSmc4Q2tAGGts8HvmDXzpFVQ6LtrVRMy1V8VzUyv/Cievb19PYk/S3gg7mVaM/bbfXTFpVUTrS1WuouGFx7eY6nz3/L/wBGvYAzV094Im2VNUt/arfXVVxo+yvht9tp6J7nIvqj5FmRO2U+6vrn6EmWbwe+H1sYxlbBrS7q3py6sviNV2E758mONO/quET6YLvACrVi8MThDYVbJHspFXSplFkr71cJ89892On6P/ElnTPGPjno2JkWmNidBW9WIiJJFp6l812EwiukVivcv1VVUkwAfDTQ2iW0qULdH2RKZGdCQpb4ehG/Lp6cY+hzN4478f8AUKq6/wCxm31yVVRVWs0zRTZVEwi/HEvohIQAr7r3gFw93Dtr7ddNhtL2tXd2VFgpEtM0bvZUdS9CL+TkVvzRSuGsOF3J7ifQO1xwk311PfbZaWrNPoHUcjauOoiRcubTtwkL3Y7dKMjkwi9MiuVGmiIAp7xj8S3ZPeynptKbjV8G3O4bJloquzXd7oaeaoavSvkTvRGoqu7eVIrZEdlqI7HUtwiuvJzglsJyctFbNqDS9LY9XSsctLqi1wNhrGTdsLP04bVM7IitlyvSruhzFXqSovG7lTupwi3Nh4g8xVnl0+2VsOmNVySK+KnpXPVkT/NeqeZQrjs5fjgVFY5MN6Yw1EB5Y9kjGyRuRzXIitci5RU+aHoAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAV55ycYdPcn9jLvp6opGM1NY4Jrppuua1PMhrGRqvkq718qVE6Ht9O7XYyxuLDAClfhN723vdvjGmn9UV8tZdNBXJ9iZPKvU+Sh8tklN1L7q1r3xJ/dib6rlS6hmD4SMP+T7fXkTsxJI9FtVxiZHG7CdP2Ksq6Z69OEwv72NFwieienY0+AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAADMfjQ5NCeL1vTpdHIyPUNvuM3l98OkmfR13V7d8K/uvbDl+eTTgzF1G1mlvG4sNar0jj1Ha0WbDFVXKthmhYn/XBH3T2T8zToAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAM1N72Mb4ye0bmtRFfYIVcqJ6r9nuKZX9ET+RpWZ4bjWhLv4zO2kisZJHbdFy1crVRVxikuTWr29FR72L3NDwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAoxYbUy7eL9qSsyxf6F2ujqfqjnSU0WO3vifPf2/QvOU/2gpW3PxLN+702VZUsukdO2tVb3bEs8Uc3Qv1Xy+rv37qXAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAHl72RsdJI5Gtaiq5yrhET5qeivPPDetNluOeoZ7V1zap1dGultNUcKdU89wrGrG10bU7qsbFfInburGp+JAOR8Opi6y0HuByKrYs1m7uurreIJnJ8SW2nmdTUsGV9WxrHMif8AMpbQjjjjtauymxGhdrJFYtTp2y09LWOjXLX1at66hzfoszpFT6KSOAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAKEbJ09RzV5lam5CX2oSt2x2UuEmntB0qoiw1N1RG+dXJj72MJKirhf3lNj+rVCY/EG31qti+Nt9qdPTvTVmrnN0xp2KHKzLVVKK18kaJ36o4vMc1cKnWkafiQ7biZshTcd+PujtrWwxNuFvoW1F3kjXKS3Gb95Uu6vVyJI5zWr/Za1O2MAS8AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAQZzU3+Zxt46ap3HpaiOO9vhS12Br8L13KoRWxKiL2d5aI+ZU92xOArW6sTmj4jMFLT5q9t+NiOkkX+FU39ZFRF+uJ4Ux7KlC72f30HKxeHdx9l2E45Wj9oIHftfrRU1LqGaZq+ek07UdFBI53xZijVqORVXEjpVT7xZ0AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAZ58ioP8AO98QPQfG6NqVeh9o4E1Tq5iL1Qz1LkjkSCRPRyKi0sOM5RKif+ypd/drcmwbPbZ6m3Q1PM1lt01bZ7hKivRqyqxq9ETVX8cj+ljU93PRPcqr4Xm2d7h201PyX1+xJdY71Xme+TyubhWUKSyeU1qL91HyPnkRE7Kx0Pb4UAuuAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAKDeKtr5mobTttxNsd7gprtunqm3w3BF/g0KVDGRueq/C1FqHxuTP8AsXeiF59NaetOktOWrSlhpWUtsstFBb6KBjURsUEMaRxsREREREa1E7JjsY66m3e0RovxYL9uHyctVybYrLeZKW0z1kDnstvkMSKgrWxM+/C1Y/MarUVUV/mYV6KaKUfiFcL66s+wwcgdOtkXv1TMqIY/XH9Y+NGev19O/p3AsQCLrRym4z36PzLRyE24qe3UrW6ooke1M4y5iydTf1Q/bPyM4900azVO++3kUbfVz9UULUT9VlAkQEK3rmrxIsCKtfyN0BJ0oiqlHfIKxe/0gc/5EeX7xRuENiYvRvC+5S4ykVBYrhIqphfxLCjPbGOrPdPbuBa0FCdQeM5xXtaPZZtM7g3qRFw10NspoYl7plVdLUNcnbP4V/T1OSj8W3cLXcax7I8L9ZaodJlI521M9QiL2/hU1K/q7qqdnp6J88IGkYM8aXe7xb908x6R45aO0FQv9Ky8Ikc8WVymW1FSrl7YRcQL3z6ZRE6Gg4t+I5uK1r93ucNPpaKT4nUujrU1HsTOehJY2UqouO2cu/xeoF65JI4Y3SyyNYxjVc5zlwjUT1VV9kOftO423t+v8ulbHrzTtxvcMTqiW20l0gmqmRNVqOe6JrlejUV7EVVTCdTfmhVu2eF9stc5WVu824+6O6lUq9Uyak1ROsD3Zyqo2LpkTKoi95FXsncnzarjZsLshKtXtTtRp3Tla+nWlfXU1Ijqx8KqirG6of1SuaqtaqorlRVair6IBJQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAACHuQ3EzY7k/baaj3Y0p9qrKCN8VDdaOZaeupWuXKtZKnq3KZ6Xo5ucrjuuah6l8EnZWse9+kt39Z2rqVyo2ugpa1rcuyiJ0tiXCN7d1VVXvn2NHQBlZJ4GTFlcsPJ9WxKqq1HaLy5Ez2RV+3Jnt79vyO10h4JOy9A1F11vBrK9SIif6sp6W3MVfqkjZ1x/i/U0eAFPtP+E7wns0bG3Db273xzEwr7hqGsarl7d1SnkiT2+WO69vTEiWHgRw402rFt/HrSU3QuU+307q7+f2hz8/qT6AOL07sps1pBWu0ntJoyyq3CNW3WGlpsYzjHlxp6ZX+anaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH//2Q==</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2020_9_20_11:17</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0526354845</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wBDAAMCAgICAgMCAgIDAwMDBAYEBAQEBAgGBgUGCQgKCgkICQkKDA8MCgsOCwkJDRENDg8QEBEQCgwSExIQEw8QEBD/2wBDAQMDAwQDBAgEBAgQCwkLEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBD/wAARCAEzATMDASIAAhEBAxEB/8QAFQABAQAAAAAAAAAAAAAAAAAAAAn/xAAUEAEAAAAAAAAAAAAAAAAAAAAA/8QAFAEBAAAAAAAAAAAAAAAAAAAAAP/EABQRAQAAAAAAAAAAAAAAAAAAAAD/2gAMAwEAAhEDEQA/AKpgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA//9k=</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2020_9_20_11:16</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>אלכס ד</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0526354845</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>328711569</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>לא</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>לא</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>לא</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wBDAAMCAgICAgMCAgIDAwMDBAYEBAQEBAgGBgUGCQgKCgkICQkKDA8MCgsOCwkJDRENDg8QEBEQCgwSExIQEw8QEBD/2wBDAQMDAwQDBAgEBAgQCwkLEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBD/wAARCAHsAewDASIAAhEBAxEB/8QAHgABAAICAwEBAQAAAAAAAAAAAAgJBgcDBAUCAQr/xABGEAACAQMDAwMCBAQBCAYLAAAAAQIDBAUGBxEIEiEJEzEiQRQyQlEVIzNhUhYkNUNEYnGRGVNylaGxFyVVV3OCg5KT0dL/xAAUAQEAAAAAAAAAAAAAAAAAAAAA/8QAFBEBAAAAAAAAAAAAAAAAAAAAAP/aAAwDAQACEQMRAD8AtTAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAB81KlOjTlVq1IwhCLlKUnwopfLb+yIi9QfqgdMuxrusPhs9LcDUtBOKx2nqkKtvTqL9Na8/pQXPKah7k4vw4AS6qVKdGnOtWqRhThFylKT4UUvlt/ZEdteeoZ0c7dX95iM7vdibnIWPuKrbYqhcZB98GlKmp0Kc6ffy+OHJfD/AML4iJHGdfnqL17Ww1jjLjZXZ+6lP8V7Ea1vWyNrNR/lzpVKkal4mo/TKUIUfqb8/BILFek70XWWmbPCZHQOUyN/bwSr5epnb2ncXE+PMpQhVVKKb+EoLj/m2G0+nHrM2I6pI5CjthqOtHJY2fFbFZSnG2vXT88VYUu5udPx+aPPHKUuG+DeJQt139N2P6IN7tOXmz2tcpawyltPL4vtqzjd4xwqdiXvrjvT+pfvwnz4kkXEdIO5+c3m6Z9vdydTzo1Mvl8RH8dVpS7o1a9GcqM6j8LiU5UnJx+E5NLlLkDcIAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAaL6les3YzpaxM6u4OpFc56pS9yz07jXGtkbnn8rcOUqUH/jqOMfD47n4YbynOFOEqlSSjGKblJvhJfuyFvUz6qOwextS80xoWo9xdW27lSlb4uuo461qrw1Wu+HFtefppKb5TjJwZEfJ7hdd/qgZW50/oHEy0NtROq6Fy4Vp0MaoL80bm67VUvqnlJ0qcexfS3Tj5mTd6XfTd2B6bVa6guMatbazouNT+O5m3hKNtUXHm0t/MKHDXKk3OouX9fHhBEWz2t9RX1FKkclulqGe1m2N21UhYSt6tnQr0Xx/SslL37vw1JSuJqD5bhL7E0unH09um/pvVrlsLpWOpdVW7jP8Ayhz0IXNzTqL9VvDj27fh88OEVPh8OciS4AEc+tDrQ0L0iaFV7eqjl9Z5enNYHAqpxKrJcr8RX4fMLeL+X8yf0x88uOc9SPUZt90w7ZX+5Gvr2LVNSo4zG06ijcZS7abhb0l58v5lLhqEeZPwj+fjcDXe7fVtvdV1Bladzn9X6vv6dnYWFsvph3S7aNrQi3xCnBNJcv8AeUny5SYfmvtwd6+rXd6Oa1FWyWrdYagrRs8fYWdGU/bhy3C2tqMeVTpR5k+F/vSk23KTve6FdmNabA9L+j9sdwalFZ2w/GXN1b0avu07R3F1Vrqipp8ScVU+px+nucuOV9TxLoY6FdHdJukKeXy1K1zO4+Xt4/xfMdqlG1T8u0tG1zCkviUvEqkl3PhKMISqAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAeLrHWmktvdOXur9c6kx2CwuOh7lzfX9xGjRpr7cyk/Lb8JLy20km3waQ6teuDaHpMwTjqO9Wb1fd0nPG6Zsa0fxNTlfTVrvz7FHn9cly/PZGbTSgBt/0/dVnqe6vp7v776lvdI7ZQqc4ylCEoUp01ynDG2snw/HiV1U57m+E6na4xDPN+fVE3L3m1O9lOhjRuUvLzIydvDULsXUvriL8Sla28lxbwXPmtW8pNvtptKRkXTN6TUauYjut1i6gq6s1Fe1PxtXARvp16TrS8t3t1z3XE/3jB9nK8yqR8ObuxHTds703aYjpfabSFvi4TjH8ZfVH7t7fTX669eX1TfPL7VxCPPEYxXCNmgdLC4XD6cxNpgdP4q0xmNsKMbe1s7SjGjRoUoriMIQilGMUvhJcHdAAEZerPr72W6Vsdc4u/wAhS1Nrj2/810xjriPvQk4pxld1EmraDTi/qTm0+YwkuWsD9RfrwsumfSs9uNur+hcbmZ625pNcTjhLWaa/FVF5Xuv/AFcH9/racUlOtDpC6Hd1etLUWT1LVzksJpe1vG8xqW/pzr1Lm5m++dOhHx79b6u6TlOKipJt8tRkGCbtbxb9dbO8Fte5qlfaiz2Squ0weAxdGcqFlTk+fZtqK57YpLmU5Nyfb3Tk+OVbJ6enp72XTFj1ububC0yO5mTt3TjCm1Uo4GhNfXQpTXKnWkvFSrHxxzCDce6VTePTX0gbJdLGDdhtrpxTy9zSVLIZ+/4rZG9XKbUqnCVOHKT9umow5SbTfl7rAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAHBfX1ljLK4yWSvKFpaWlKde4uK9RU6dGnFNynOT4UYpJtt+EkByznCnCVSpJRjFNyk3wkv3ZXH1b+p5fLUb2H6NrB6s1hfVnYVM/aW7u6VKs+U6VjSSauKi4bdVp04peFPnujr/qc6s92+uXcmr0m9HNK7lpes50c7naUnSjkaEZKNSpUqpc0LBNpN/mrdyjw1JQlM/o/6HdrOknTqniKMM9rW9o9mU1LdUFGtNNLuo28fPsUOVz2puUnw5SlxFRCOHSZ6XNWnnlvd1j3y1fq6/rfj1p+6uHeUKdaXnvv6sm1c1OX/AE03TXHl1E+FY1QoULWhTtrajClRpQUKdOEVGMIpcJJLwkl9jkAAAACLvXT1uaX6R9DKhjvwmW3BzlKSwmHnPmNKPlO8uUnyqMWnwvDqSXamkpyj7vWh1haN6R9t5Z2/9jJ6ty8Z0dPYT3OJXNVLzWqceY0KfKcpfduMV5lyqaNoNod+PUK3+yF9eZO5vbzIXEb7Uuo7uLlbYy2b4SS+Oe2PZRoR457Ul2xjKUQ7XTP067t9fG+l/kM/m7+vaVLqOS1jqi5alKjTnL8kOV2utNRcadNLtio88KEHxfZtttvozaPRGJ272/wlHFYLC0Fb2tvT+ePvOcvmc5PmUpPy222eLsVsdoDp422xe2G3OLVrjsfDurV5qP4i+uWl7lzXkku+pNpcv4SSjFKMYpbAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAGKbobp6C2Z0VkNwtytSWuEweNhzVuK8vM5v8tOnFfVUqSfiMIptv7Ae7nM7hdM4e81BqLLWmMxmPpSr3V5d1o0qNCnFcuU5yaUUv3bKpuozqh3U9Qzcel0qdJdjeUdF1av/rzOVO+jTvbeMl3V7iXHNCzg+Gov66su2KTlKNN+HqncDqQ9WPcytoHba1vNG7M4O6hO9q1/FOMOfpq3bi+K9zJeYW8ZOMPnnw6hZp099Om2HTPoGhoLbLCQtqX01L+/qpSu8jXS81q9T5k/L4j+WKfEUkB4/Sz0q7bdKO3lHReh7f8AF5K5jCpm85XpKNzlLlLzOS5ft0021Ckm1BP5lJynLc4AAAADWnUTv9ofpq2ryu6eu7hu2sYqjZWVOaVfI3k0/atqXP6pNNt8NRjGUn4izPM9nsNpfCX+pdRZO3x2LxdtUvL27uJqFKhQpxcp1JyfwlFNt/2KU94Nabq+qh1TWWhNs6Ne10NgJzpY6pWhKNDH2PelXyVyn/ravbHth4fCpwS57pMNcaR0V1Bepv1J3+bvbhxdeUJ5TJzhJ4/TuNUn7dGnFv7LuVOkn3VJ98m/NSorvththduenLbux222zxH4TH2v8y4uKrUrm+uGvrr158LvnLj+ySSjFKKSXX6eunvbrpo22sdtducc6drQ/nXt7W4dzkbppKdxWkvmT48JfTFJRikkkbMAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAGq+pDqQ246X9uLrcTcS/fam6GNxtBp3WSuuOY0aMX/zlJ/TGPLf2TDt7/8AUFtp017eXm425uZVraUeaVnZ0uJXWRuWm429Cnz9c3x8+IxXMpOMU2qutH6K6hvVq3blrrcC9utIbP6dupUqFG3cpULePHm3tO5dte7ku33a8lxFST44UKTbObL72+qZvHU3032u7nC7YYeu7e1t7fup06lKM+XYWHP91/OuHy+fHmXChbtpDSOmdA6YxmjNG4S1xGEw9vC0sbK2h206NKK8Jfdv7tvlttttttgebtlthoTZzRWO2+2405aYTB4umoUbe3hx3S4+qpUl81Kkn5lOTcpPy2ZUAAAAA6eXy+K0/irzO5zI22Px2OoVLq7u7moqdKhRhFynUnJ+IxjFNtvwkj9y2WxmBxd5m83kLewx+PoTubq6uKip0qFGEXKc5yfiMUk22/hIqA6nepvdb1FN2rbpe6Y7W8/yG/Fd1zcNSowycKU05X15JrmlaU2lKEJJOUnBuLqOnCIcnUr1L7t+ozu1Q6Y+mOzuqeg4V+67upqVGORhTmu6+vJcc0rSD4cKbXdJ9rac5Qpwsd6U+lbb3pP24paJ0bTd5kbtxuM3ma0Eq+SuUuO58fkpx5ahTXiK/eTlKXD0m9KG3/SbtzT0fpSnC+zF721s5nKlJRr5G4S8c/LhSjy1CnzxFNvzKUm93gAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAADVvUf1FbfdMW2d9uVuBdydOl/Ix+PoyX4nJXTT7KFJP7vjmUn4jFNv44YfPUf1IbbdMG3V1uFuLke1fVRxuNoyTusndccxo0Yv/nKT+mK8t/HNZmyeyG8nqh7zVeoDf64u8VtdjLiVCys6FSUKdelCf8Ao+y+6gmv51x+ZvlL6v6fZ2W2M3l9TzeGXUH1C1rvF7XYyu6OPx9KcqULijGXP4KzS4cafK/m3H5m/Cbl5hbbp3TuC0lgcfpfTGJtcXicVb07SysrWmqdK3owiowhCK8JJJID803pvAaPwFhpbS2ItcXiMXbwtbOztaahSoUoriMYxXwj0gAAAAHXv7+xxVjc5TJ3dG0s7OlOvcV601CnSpQTlKcpPxGKSbbfhJHJXr0LWhUubmtClRpQc6lSclGMIpcttvwkl9yozrR6udfdaO5dt0h9KlG5yGnru8/C5C8tn2rN1qcuZTdT9FjS7e9yfCn29z+lR5DpdWXVRuZ197q2vSr0t211W0dK6Ubq7pylSjmPbmu67uJcJ0rKl4koyXMmlJpycIRsP6Rukjb/AKSdu46W0xFZHPZFQrZ7O1aajWyFdJ8JL9FGHLUKfPhNttylKT6HRt0c6F6Rtv44bFKhldW5SEZ5/Pul2zuqi8qlT58woQ54jH7vmUvL8SEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAGNbjbjaL2l0Xldwtws/bYbA4ai691dV34S+IxjFeZzk2oxhFOUpNJJtgdTdrdnQmyGgMruVuPm6eMwmIpd9Wb81K03+SjSh8zqTf0xivlv7Llqo7R2G3W9Wjqfqak1a73A7VaTqKVahTquULCycuYWlGXHbK8r9v11OF2xUpcNQhTliu5e52+fqp9ReN270RZ18RpCwq1KuOsazbt8VZJ8VMjeuHiVZxaXHLSco04P6nKVw+wWxWg+nLbHFbW7eWHs2FhH3Lm5qJe/kLuUYqrdV5L81Sfav7JKMVxGMUgzHTWmsBo3T+O0ppbE22Lw+JtqdnZWdtBQpUKMFxGEV+ySPTAAAAAAVleoN1u6k1vqeXRn0tfiMvqLN3Kw+eyWObc3Vk3GeOt5fCf8A11VPtjHujyuJuIY315dZutOobXcejbpLd1mKWSuXjc3ksXPl5ar59y0o1F4jawSbq1uVGajJc+0m6kw+iPop0b0jaE9qStcvrvM0oyz2cVN+furW37vMKEH/AGTqSXdJL6Yw8joO6GdMdJui45jOUrTK7kZu3j/GMpGPdG0g+JfgrZv4pxaXdNcOpJcvhKEYytAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH42opyk0kly2/sB5Wq9Vac0NpvJaw1dmbbE4XD207y+vbmfbToUYLmUm/wDyS8t8JJt8FH3Uz1E7u+o/vxiNqtpsNff5MUb2dDTeF5cVU45U8letcqMuzmTb5jSp8pctzlPOPUp6zMv1G7g0emrZKvXyWk8bkqdnXljlKpLUeW71GMIdv9SjTqcRppeJ1OZruSptTv8AT/6J8L0o7eLL6itre73H1Lb055u9SU/wVP8ANGxoy88Qg+O+Uf6k1y+YxgohnfSB0m6J6Stsqej8A6eQz2R7LjUGbdPtqZC5SfCSfLjShzJQhz4Tbf1Sk3vUAAAAABBfr2648zt/kKPTT03wq5zd3UkqdnOWPh708PGsvpjFLlfipJpxi/6cWpy/TyGP+oJ1xagxmYXSb0vyucxuTqCrHG5S9xadSrjfcXDtKDX+1ST+qfPFGPd8T809mdA/Qbp/pV00tXaujbZbc3N26jkb5cVKWNpS8u0tnx8fHfU+ZtePpSR89B/QdhumPDT19uBUoZ/dXPU3PIZKcvejjY1PM7e3nLy5Nt+5V+ZvwvpX1S+AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAVj+pV6jGKweLzPTlsPmI3eZu4VLDU+obSrzTx9N/TUsreUfz15LujUmnxTXMVzUcnS871IfUkeNeU6fOnjUDV4nO01Lqeyq/0PtOztKkf1/KqVU/p8xi+7lxw700PTulrWrjeorffBNadpSjdaYwV1D/Sck+Y3lxB/wCzp+acH/UaUn/L49wNnelL0PrRuJtOpzdPD8Z7K0HLSlhcQXNhaVI8O9kn8VasW1D/AA05N/M/pssPxJRSjFJJLhJfY/QAAAAES+uLrOnsRZWe0W0lg9R7x6yjG2wuLt6fvOwjVfZG5qwXzJvn24P5a7pfTF9weR1ydbGT2nubTYLYGylqPeTVbja2dtaU1XeKVXxGpOHw6zT5hCXhL65/SuJer0OdDOM6bsfc7j7j3kNTbualU6+XzFao6/4J1X31KNGpL6pSlJt1Kz+qb5/T89vom6LLXp7x91uVuZkf8qd39VxdfOZu5m68rP3OJTtaFSTba5/PU+ZtL4ioolWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAra9Tr1A3t5aZDpz2UzfGqLyi6Gpc1aVFziqM01K0ozXlXMo/mkvNOLST73zT2J6jXX1ZdOGnq21e2GRoXO5uZt+J1I8TjgLapHxcTXw68k06dN/HipJdvbGdbPRD0eav6x90qt7nri/oaLxVz+L1RnajlKrcTk+/8NSqS577iq3y5Nvsi3N8vtjMNnemp0FT6gdQUt491cVNbcYS4/wA0tK0Gln7uEvNNc/NtCSaqNeJSXtr9fbdrb29vZ29K0tKFOhQoQjTpUqcVGEIJcKMUvCSS4SR52ldLad0RpvG6Q0liLbFYbD21OzsbK3j206FGC4jFL/gvl+W/L5Z6oAAAADUXVF1KaI6Wdqr/AHI1hNXFx5tsPi4VFCrkr1xbhRi/PbHxzOfD7YpvhvhMMC64us7A9KGhaNviKFDNbiaji6OncJy5vlvt/FV4xfd7MZeElw6k/ojxxOUMH6D+j3UWhLq96mOoutcZreTWffdVJX776mFo1fmklz2xrSjwpcJKnHilFRSl3af9P3YLWvUduVedenUunkr28upS0hj7mn/JjKnJxV1CnJtQpUWnChH/ABKVT5jCUrMgAAAAAAAAAAAAAAAAABjGtt0NtdtbNZDcTcDTmmLdpuNTL5SjaKfH2j7kl3P+y5YGTggxvD6vvTFt+q9ht/SzW4mTp8qP8PoOzse5fKlcV0pcf71OlUT/AHIyXHqD+oZ1O3FfF9OO08sLjqtSVON1g8LO/qUV941b25Tt4Ph8dyhTa+3D4AuCBT5R9Pv1K97H/Et3d5nilUXdK1z2sLq7lDw+Iwo2qq0Y+fspRXlvy/ByR9GfqN07J32i9+dKUb5ruc1Vv7Jua+Prp05v7vzx9/gC38FQ9Lo+9WzQKja6V3ty2Tt6KSp07XX1edGK5fiNO7cEl55f0rnk62stFesboTR2b1jqHX+bhicHYV8lfzoagx9arC3owc6koxg3OTUYt8R8+PHkC4EERfTL6l871G9P05a71DLL600lkauNy1xVjCNa4ozbq2teSglHhwlKlzwm3Qk3y+W5dAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAiN6gfXLjOk7RtHTulY0L/cfUttUlibefbOnjqKfa72vDnlrnlU4tcTlCXPiEkba6pupXRfSxtNkNydWSjc3XP4XD4qNRQq5K9kvopR/aKXMpy4fbCLfDfEX/AD9601lun1T71VM/m6lbO6y1tk6NpbW9JcR9ypJU6FvSj+inFOMIr7Jctt8sDYPTV027vdcu8l655O9rUKt1/EdWapvuaqt41JNyk5P+pXnxJQp/dpt8Ri2r8NotpNCbG7f4nbPbjDQxuExFLspx57qlao/M61Wf66k5cylL9344SSWP9NGwel+mvZzAbWaat6DqWNCNXK3tOmoyyGQlFe/cSfHL7pLiPPLjCMI/EUbSAAAAAANMdVHVTtz0nbdz1vrmrO7v7xzoYTCW81G5ylzFJuEW01CnHui51GmoprxKUowlWvtbs91HeqTutY70b53Tw+2GEuPZtqFKEqFvK3VVSqWdhBPulKfxUuZNv6UnJ9kIR8bdXOWXqI+pFhtAWWRubvb/ABd48RbzoTcYyxllCda9rQkvEffnCqoVPnidH9ki5jAYDCaVwljpvTeKtcZisZbwtbOztaSp0aFGC4jCEV4SSQHJhsPitO4ex0/gsdb4/GYy2pWdnaW9NU6VvQpxUKdOEV4jGMUkkvCSR3AAAAAAAAAfjainKTSSXLb+wH6DSu6HWf0ubOwrR1zvXpqjd0ee6wsbn8feKS/S6Fsp1Itvx9SS/v4ZDjdn1sdBYv8AEWGy+0+VztZNwpZDPXEbK3T4/OqNPvqTjzx4cqb4/YCzE1vup1H7EbI0J1d1N1tOaeqwg6is7i8jO8qRXy4W1PurVPt+WD+V+5TplOrD1GOs3I19PbdT1LHHXMpQnYaJsJ2FpQj47o1bxP3IwacU1Vr9v1cfq4ewdqfRo301rVjnN7dwsRo+NzJ1a9tQby+Rcm+X7jjKNFN+fqVWf/BgSH3K9aTYLTc69ptroHVOs7ik+Kdeu6eLs6394zn7lZf/ADUURr1X6xvVFra8/g+2W3+lcDO5n228KFlXyd839knKShJ//SJsbX+lB0g7e0KNTO6VyeuMhT4bus/kJuHd8vihQ9ul2/2nGfj7vy3KPRm2u3W3Np+B2/0Fp7TVu49jp4jGUbSMl4+VTiufhfIFPGMxHq9dS1R062R3IxNhcrmrWu60NL2vtvx+SKoOpHz8QjJteeGvJsPQHosbhajvf47vvvnY29xcT925o4WhVyFxW5X6rm49tRl+77Jrx9/ktoAEW9m/TV6SNm40rqht1T1dlafD/iOqpRyEuV8NUXFW8Wn8NU0/jz4JPWdlZ461pWOPtKNtbUIKFKjRpqEKcV8KMV4S/sjmAAAADiurW3vbatZ3lCFahXpypVac490ZwkuHFp/KabXBykVvUd6nH029Pl+8DfOhrDWXuYXAuDanQco/z7pPjw6VOX0v/HOn9uQIBdGGVjsn6mWT2p2UzlfOaIy2XyuBuIQ57KtlRp1qsZNt8SdvUp8Kr+uMJuPCqcF0xUz6LewLvs3qnqPzlm/YxsJacwLnHw7iajO7rR/vGm6VNNeH7tRfKLZgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAHk6s1TgND6YyustV5OljsNhLOrf393V57aNClFynJ8eXwk/C8v4Xk9YqB9VnrjjrbJ3/S7tfkITwGKuoLVWRoz5/HXlKXP4KDXh0qU1Fzfy6sElwoPvCI/WH1Sao6rt377XOUlXtcDZSnZ6cxU5fTY2Sl4bSbXu1OFOpJc8vhJ9sYpT99KDofq6Zs7Hqo3PsHDJ5G2k9I42tTX+b2tWKX8Qnz5U6kHKNNeOKcnPz3x7Yc+nT0prqe3zoR1LYzq6I0gqeUz7cX2XP1fyLPnjj+bOL7l/1cKvDT4L/KNGlb0oUKFKFOlTioQhCKUYxS4SSXwkgPsAAAAANS9W1hq3J9Me6Floa7nbZuelsg7adPnvko0ZSqQg001OVNTjF8+JST+xto4by0tr+0r2F5SVW3uacqNWm/icJLiSf/ABTYFPvok4rSN1vDuDlchCctS2OnqEcWvmEbSpccXcv+13RtUn+0p/uXEH8/26u1PU/6de82R1JpC4y+nbGtXuLHB6os6cK9pkLCU4zhSm5xlDv4jTc6VRc90G0mkpPdGifWo34wmAeO1ptzpTU2ShJe3kYSq2LlDjz7lKHdGUuefMexf7oFzIKgP+m93T/9x+lf+8bn/wDR26Xrg6+jaThX2C0/O5afZUhmq0aaf25g6bb/APuQFuh8znCnCVSpJRjFNyk3wkv3ZSdrr1luqHUdKpa6PwGjNJU5R4jXt7CpeXMX+/dXqSpP7f6r9/n7a0xeO9QnrnuY26vNf6uxF1Lida6rSsMDDjhtv+naKSTT4inNr4TAuO3L63OlPaX3Kest79NK6pJuVljbh5G5TXjtdK2VSUW34+pL/l5Ip7i+tfs3hvettsdq9Uamrw+mFfJ16OMt5v8AxRcfeqNfHiUIt+V4+TX21nojX1ahQvt6d6KdtVlHmtjdNWXudr58cXVfhfHHP8j5b8tLlyw249MDo127hRqT2ynqm9o8f53qO+qXjnx/iopxt3/+ICvvVHq29Y25t68HtdpzA6frVk1Rp4TCzyN9xz8/z3UjJ+V8Ul8niS6evVG6pVxre33Bni7nn3Keqcs8VZwTfl/g6s4fv+mi/C/sXZaW0TozQ1gsXorSOF0/ZJJK2xdhStKS4+Popxiv/A9oCpbbL0RtTXTo3e8O9OOx8fDq2OnbGdzN/wBlcV/bUWv/AIUl/wCZMbaj00uj/aapRvbbbKGqMjRUeL3U9d5Btryn7LSt0+VzyqSZKMAdbHY3HYexo4zE2FtZWdtBQo29tSjSpU4/tGMUkl/ZI7IAAAAAAAAAAA8/P5/C6Vwd/qXUeUtsbisXb1Lu9vLmooUqFGEXKc5Sfwkk2Bi29W8uhNg9uMtufuLlY2WJxVLlQTTrXdZ8+3b0Ytrvqza4S/4ttRTaoY3d3V3v9QXqGtKWPxV1f3+VuXYabwFvJyoYy1b5a5+IpRXfVqvheHJ8RSSyTrc6t9Y9aW8Ftp/RlrkZ6Px96rDSeDo0pSrXtacuxXM6S5cq9VviMePpi4wXnucrQPT56HcR0raGjqbV1pb3e5eoreP8VufpqLG0W1JWVCS+y4i6kk/rmvlxjEDeXTds1jen7Y7R+0eN9qUsBjYU72tTbcbi+m3Uuqy588TrTqSSfwml9jZQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAhx13+oTpLpbxVxoXRcrTPbn3lFe1YyfdQxEJwUoXF1x8tqSlCinzJNN9sWnIPD9S7rjt+nnRNXajbjLRe5Gp7VxdahP6sFYzXEriTXlVprmNJfK81Hx2xU6uukTo93I6vtfSxWElVxum7Coqme1HcUZVKVrFvnsh8e7cST+mnyv8AFJqKbPc6aemPejr53fyeoc1m7946pefi9V6uvour2Sn59umnwqlaSSUaa4jCPDfbFJO9zabafQmyOgsXtttvg6WLweJp9lKnHzOrN+Z1as/mdSb8yk/l/suEg6OyGx23HTzt7YbabYYRY/E2XNSpUm1O4vbiSSncXFThe5VlwuXwkkoxioxjGKz4AAAAAAAAADzNSaa09rHA32l9WYSxzGHyVF295Y3tCNahXpv5jOEk01/x/YhxeekD0eXWZr5SnY6wtbetUlUjj6Ob/wA3pJ/oi5U3V7V9uZt/3JtACFX/AEQ3Rt/7F1X/AN/VP/5Puj6RPRpTqwqT0/qirGMlJ0556qozSfw+Enw/7NP+5NIAaD256DukXaytTu9K7GaeqXdLhxustGplKqkl+eMruVTsf/Z4/twb5o0aVvShQoUoU6VOKhCEIpRjFLhJJfCSPsAAAAAAAAAAAAAAAAAAAAKe/Va63amuc/d9Mu1+X505hLjt1Te0J+MhfU5c/hIyT80qMl9f+KquPimnKTnqX9c1Dp+0dW2j2zzMf/SRqO34q17eacsFZTXmtL/DXqR5VNeHFN1PHEO6EXpn9ENbqI1zHdncfFuW3WlrtS9qvHmObyEGpRtuH4lRh4lVb8PmNNc90nAJMelR0Nw0dibPqb3Ww3GfydFy0pj7mHmwtZx4/Gyi/irUi2of4abb+ZrtstPmEIU4Rp04qMYpKMUuEl+yPoAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABA/qZ9K/B9R/UTeb3Xu715hcfnXYvM4mniY1q0lb0KVBqhcOqlT76VGK5lTn2y5lxNPtU8ABi22e2OhNndF47b3bfTlrhMFi6fZQtaC+W/Mqk5P6pzk/Mpybk35bMpAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAARW66eufSPSXpB4rFStsxuNmreTw+IcuY20HyleXSXmNKLT7Y+HUknFcJTlHxOu31CNH9LWIr6J0ZUss/udeUE6GPb76GJhNcxr3fa/njhxo8qUk032xabrh6XOkHe3r93KyG6u5efytDTFe997PaqvI81r+omlK2s012ymort5S9ujFJceI05B4fSv0vbtdfO82S1brDMZOWA/HfjNW6puH3VJzl9X4ag5JxlXlHhRil20ocNrhQhK+DQuhtKbaaQxOgtD4W3xOCwltG0sbOhHiNOmv/ABlJtuUpPlyk22222dTbLbHQuzuisbt7txp22wuCxVP27e2o8tt/qnOb5lUnJ+ZTk3Jvy2ZSAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAr/8AUP8AUdttjKF1s9sbl7S73CqP2snkoxhXpYKDT5ik+Yyuvj6ZJxgnzJN+F8eot6jFnsna32ymyeUpXW4FxD2spk6TU6eBpyXmEX8O6afhf6tPl/VwjWPp1+nRd5a5sepXqSxtW4r3dRZPAYC/i5Tqyk+9X14peW233Qpy8+e+X6UBgvRd6aGtt9c1T3z6qZZe209kqzyVPG3teospqCpOXe61zOX8ylRm3y5N+5U5bXampu3vT+nsFpPCWOmtMYezxWJxlCFtZ2VnRjSoW9KK4jCEIpKKS+yO+kopRikklwkvsfoAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAACv31F/UWtdkLW+2T2WyVK53AuqLpZPKUpKcMBCS/LH7Sumnyl8U01J8vhHc9Rn1DLLYTG3Wzez+ToXW499S7L+8h9UMBQnH83Pw7mSf0x/Qn3y/SpaX9N708rzUl7YdTfUXjK9enWqrJacweRjKVS8qt98chdqfmUG33U4S572++X09qmHb9OX06rrLXVj1K9SWKndzu5LJaewORTqTrzm++N/eKXPdy33Qpy5bb75fZO1MAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABCL1E+v7HdNmAq7Y7ZX9tebm5i35c4uNSGBt5rxXqp8p1pLzTpP+05Lt7VPJ+v3rlwnSfotaf0xVtchuVqChJ4mxmu+FhRfMXfV4/HammoQf55J/MYz4hj6fvQln+ozVE+qLqZpXeR0/eXksjj7LIpTnqS6c25XFdS/2ZSXHa1xVfjxCPEw9j05fT+ym5GYt+qLqRsLm9sbq5eUwmJyilOtl7iUlU/iF33+Z0nJuUYy591/VL6OPctrSUUoxSSS4SX2PyEIU4Rp04qMYpKMUuEl+yPoAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABH3rO6vdH9I22c9R5FUMjqrLxqW+nMJKfDu66S5q1EnyqFPui5yXHPMYppyRl3Un1F6B6Ydr8huVru7T9pOhjMdTmlcZO8abhQpJ/vxzKXxGKlJ/BVh067B7reppvtk+oLfm7ubfQVldxpXHsylTp140+HTxVkueadOMZL3Ki8rub5dSo5IOfov6P9wOuHc6+6nepS7vbvSVe/lc1HcqVOpqG4i+FQopcdlpT4UJOPjiKpQ+JOFy1lZWeOs6GPx9pRtbW1pRo0KFGmoU6VOKSjCMV4jFJJJLwkjrYHA4XS+FsdN6cxdtjcXjLenaWdnbU1TpUKMIqMIQivCSSSSO+AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAxPdLdHRGzOhMtuRuJmqWLweGoutXrS8ym/006cfmdST4jGK8ttHsan1Pp/RensjqzVeYtcVh8Tbzu729uqihSoUYLmUpN/bj/n8Iqh1Hf7qerdv5/k5putf6a2G0Ld91S7ce11H9SVdxl4neVYNqEHzGjTbbXLl7gY3pLR+73q19RFbX+s43um9pNK1Xa0oUppxs7duMvwdvJx7al3VXbKrVaaiu1vwqUHb5ozRul9vNK4vRGisJbYfBYW2haWNlbR4p0aUV4Xnltvy3Jtyk22222zpba7a6J2h0Ritu9vMDb4fA4aj7Nra0V+7blOUn5nOUm5Sm+XKTbb5Zk4AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAADiurq2srate3txSt7e3pyq1atWahCnCK5lKUn4SSTbb+DlK9t/tzNf9eO5l/wBJvTbmXYbc4arGnuFriku63rJS+uztpJpVY+HHhNKrJPyqUe+YYNu7rjcT1QN5Z7CbI5e5wux+kbiNXUupYU32ZOrGT7ZJNr3I8x4o0vHL7qs/Cj2WJbS7TaE2Q0BittduMJTxmExFLspQXmpWm/M61WfzOpN8ylJ/Lf2XCXX2a2Z282D2/wAbtrtngoY3D46Py33V7qs/z169TjmpVk/Lk/7JJRUYrOAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEbusTqRzm1eMw+0eztnHNbybj1JY7S+NhHv8AwcX4q5CuviFOlHuknP6W4ttOFOpwGC9Se5m4nURuXfdGHTpmHjI0LaM9x9Y0X3QwtnU8OxpNPzcVI8qST5SbjyuKjjI/ZPZTb7p/28xu2m22GhYYvHx5qTaTrXddpd9xWn8zqSa8v7JJJKKSWO9L3Tvgum7bG30haXbyuocjWllNT52ry6+XylX6q1ecpee3l9sIv4ilzzJyk9vAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAMc3F3B0ltTofM7i66y1PG4HA2sru9uZ+e2C4SjFfMpyk4xjFeZSkkvLAwvqW6itGdM22V3uBqtzurqpNWWFxNB83GVv5p+3b00k3545lLj6Ypvy+E9W9HHT9rjEZPNdT3UVxebvbgRUp29SP0abxb4dLHUYtvsaSj3/ddsYvlqcp696X9Dau6vd3KXXHvjiJ2WncbKdvtVpa4fdCyt4z/wBJVI88OrJx5jJ/M13riMKDU6wAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAV067y156kXU8tndNX1SWwu0d9C71Te0J8UtQZOLlGFCEk+ZU241IQlF8dirVE33UjY3qNdR2o9Hadw/TPs0q13uhuxJYu2hayaq4+wqy9udbleYzqPupxl47YqrU5i4LnefSr08ac6YdlcHtZgvbr3dCH4vM38Ydrv8jUS96s/7eFCCflQhBcvjlhtaxsbPGWVvjcda0rW0tKUKFChRgoQpU4pKMIxXhJJJJL4SOcAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA1pV6c9oq++lLqPr6WVXXlDG/wALpZCdepKFOl2uHfGk32Rqe3KUO9Lntk192bLAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAD/9k=</t>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wBDAAMCAgICAgMCAgIDAwMDBAYEBAQEBAgGBgUGCQgKCgkICQkKDA8MCgsOCwkJDRENDg8QEBEQCgwSExIQEw8QEBD/2wBDAQMDAwQDBAgEBAgQCwkLEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBAQEBD/wAARCAHsAewDASIAAhEBAxEB/8QAHgABAAICAgMBAAAAAAAAAAAAAAgJBgcFCgIDBAH/xABCEAACAQMDAwMCAwYDBgMJAAAAAQIDBAUGBxEIEiEJEzEiQRQyURUWI0JhcSQzUhcYJUNigTSCkSZEU1RjcnOhsf/EABQBAQAAAAAAAAAAAAAAAAAAAAD/xAAUEQEAAAAAAAAAAAAAAAAAAAAA/9oADAMBAAIRAxEAPwC1MAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA8K1Wlb0p169WFOnTi5znOSUYxS5bbfwkgPMGLX+6u1+KnUp5TcjS1nKk0qkbjMW9Nwb44T7prjnlf+qOG/3iOn/wB6lb/7c9vvdry7aUP3nsu6cv0ivd5b/sBsIGL0d09sbirChQ3G0vUq1JKEIQy9u5Sk3wkkp+W2ZJQr0bmjC4tq0KtKolKE4SUoyT+GmvDQHsAAAAAAAAAAAA4zUuptOaNwV5qfV2ex+Fw+Op+7d3+QuYW9vQhyl3TqTajFctLy/lpAcmDgtF660XuPp+hqvQGq8TqPDXMpRpX+Mu6dzQlKL4lHvg2u5Pw18p+Gc6AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAADhda6wwG32kM1rrVN6rTD6fsK+SvqzXPZQpQc5tL7viL4Xy3wvuB69ca80Ztppm91lr7U2PwOFx9OVS4vb6uqdOKSb7Vz5lJpPiEU5SfhJvwV+7retXtLgZ3FhtBtlntV16dSVOF9lK0MZaTSbSqQilUqzi/DSnGlLz54IC7kbodRHqF7+UMFj5ZLLV8tf1Vp3TcLlqxxFtx5ai2qcO2lFOrWaTl28t/CVgGxXoy7R6exNlk9/NT5TVed8yusdirt2mLjzzxBTUFcVOPD7lOn5/l4Ahlub6pHWPu1XeIwOq7bSFrdz9qnY6VsParzbf0pV5upcd32+icef0+xjGP6TOvzqCqLL5TbncXPSrz91Xeq76ds6j7ee9TyFWDl4fiS55+FyXnbX7AbKbLW/4fava/Tum5OChO4srKCuasf0qV3zVqf8AmkzYAFE1h6RvWdd04zuNM6asXKXa4V8/Rbiv1ft9y4/s+f6HMP0cOrrmC/GaCff8v9tVfo8ff+B/28cl4IApEh6NPVrOE5yzO3kHFLiMsxccz/txbNf+vBjt90R+ov011aud0DhtV0qVF90rrQuelWnV8/H4ehNV5r9U6TTT8/cvdAFJenOuX1P9uParam09qXNWVtFfwdR6EnGDivnvq0qNGrL5XLdTn48m9tpfWtwda5p4ffzaC8xFaM/ar5HTtb3qcJfD7rSu4zgk+eeKs5cfytrzZ8a53X6ddjt8rSVpuvtfgNRSlHsjdXFsoXdOP6QuafbWp/8AlmgPj2f6oNgd+reFXardHCZu4lBTlj1W9i+pr/qtqqjVS8Pz28ePDNpFZW+Pox6cre7qbpr3GvsBlKEvft8RnajrW7qJpxVK7ppVaPHHKc41Xzx9UV5NK4vrI9QfoYzlDRu/+nb7UuGcuyhDU/dce/FLz+FylJt1Hxx4nKqor+SLbAufBDDYD1WOmjeSVthtX5CttvqCvxD8NnasXYznx8U71JU0vtzVVLnjwvgmXb3Fvd29K7tK9OtQrQjUpVaclKE4NcqUWvDTT5TQHsAAA1B1ZbCvqW2E1Ps/Rzn7Iu8tTo1rK7lHupwuaFWNakqqSbdOU4KMuPKTbXLSRt8AUM9LXUpux6eG+eX243PwmSp6elextdVadnJOdCfC7L2289rmoOMk4vtrU+1c/klG87SOrtM6+0xjNZ6Nzdrl8JmLeF3Y3ttPup1qUl4a+6f2afDTTTSaaIw9f/Q3heq7RH7waWoW1juXp+3axF7NqnC/opuTsq8v9Lbk4Sf5Jv5UZT5rs6EetrVnRtuDebNb0W2SpaEr5GdrlLOvSnK503fKXbO4p0/MnDuX8WlFctLvgnJONQLyQfFhc1iNR4iy1Bp/J2uSxmSoU7qzvLWrGrRuKM4qUKkJxbUotNNNeGmfaAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAgH6yG8f7k9PWK2psajjfbiZNRrcPjiwspU61X+vLqytV/VORPwqR9cPG3dLWe0+XnObtbnF5W2pxb+lVKVW3lNr+rVWHP8AZAen0UtmLnJa01nv1krLmxwtmtN4yrOL7ZXlZwq3Dg/jup0o0ov+lz/Ut0IIejPkqV90l5O1p0VCWO1pkLaclHjvk7a0q8/18VUuf6f0J3gAAAAAAAAAAAOH1Zo/SmvMBd6V1rpzG53D30ey5scjbQuKFVfbmE01yn5T+U/KOYAFaXUv6N2jtRQutT9NGfWm8k26j07l606uPq/dxo1+JVaL/RT9yLfC5gvJDTRe+vWr6eGtIaGzdPLYqxo1JTlpnPwdzirympcSnbSUu1Rb/wCbbzXLXlvhov4MR3Q2k233p0pcaJ3R0fjtRYe5TboXdPmVKXHHuUqi4nSmvtODjJfZgR46UPUi2P6l1Z6YyFytF67rpQ/YeSrL2rup9/wlx4jV/pCSjU+eItLuJalNfVp6R+vNuXea56cLi91hp6n3V6mCq8PLWUfnik1wrqK+yilU+F2zfMjhOlL1UN2ti7yjt7v3a5PWml7ObtJVbmTWbxTi2nFTqNe+ovlOnVakuElOKj2sLrwYRtDvTtjvvo+hrrarVtnnsTWfZOdFuNW3qceaValJKdKa/wBMknxw1ymm83AEC/Un6BKG/mCuN59psRCG5GIt072zox4/eC0px8Q4XzcwikoS+ZxXtvnin2z0AFIXp3df2T6as9DZzd+4uqu3N/dOEKtZTlW03dSm++pGHDboSk26tJLmMvrj5741LtrG+scpZW+Txl5Qu7O7pQr29xQqKpTrUppSjOEo8qUWmmmvDTKyfU+9PqOoKGV6l9ksL/xWjGV3qzCWtNJXdOK5nf0IJf5qS5qxX51zNfUpd+p/TO9QWptTk7Hp/wB6s3KWisjWVHBZe6rfTg68nwqNWUn9NrNv554pSfL+iUnALlQfiaklKLTTXKa+5+gAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAACrP1y7GvUsNmclFL2aFbUFCf691SNg4//AKpyLTCFPq17P325nStcanw1pKvkNAZKlnpRguZysuydG5S/pGNSNVv9KLAwf0TspTrdOutcIpQ9y01rVupJP6kqtjaRXP8AT+C+P+5YcUt+jXvPT0Xvzm9osnc9lluDje+0UpeP2hZKdWCX2XdRlc8vxy4wXnwXSAAAAAAAAAAAAAAAAACLvVx6fmzXVRY3Gbq2kNLa8VP/AA2o7ChHurySajC8pLhXEPjy2qi7YpTSTi5RADrz6n0b1X+nNu7Rv6d3f6ZyEnKNllrGTrYrN28WnKH1Lsrw8xcqVSPdBuLcYvtZZx0ceqFtp1BVLDQO59K10Tr+v20aMJVH+zMrV4/93qSbdKbfPFGo+fMVGc2+FLrcbbTQe7mkr3Qu5OlrDUGDv48VrS8pKcVJc9s4P80Jx55jOLUovymilzrm9NjWHTbO63L2tlfal2473Urza777B8vwrhRS76P6Vorx8TUX2ymF5IKlfT49Tu5wlbF7H9SmdnXxk+yzwerLupzO0fhQoXs35lS+0a7bcPCnzH64W0U6lOtTjVpVIzhOKlGUXypJ/DT+6A8in31OPT6/2f3eQ6i9ksHL92LqpK51Nh7aLl+y60pcyu6MV8W8m+ZxXinLyvofFO4I9V1a217bVrK9t6Vxb3FOVKrSqwU4VISXEoyi/DTTaafyBV76WXXvHJ08d0v7z56MbynGNto3L3dT/wAQviONqzb/ADr4oN/mS9rnu9qMrRykT1GegfIdOWoau820llVlt1k7tTqULfudTT11OX002/n2JS49ufP0tqD4fY5zD9Nv1ArXffC2uy272ZhS3GxVDssL64ml+8NvBP6k/wD5mEV9cfmaXuLnioohPgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA+XK4vHZzF3mFy9nSu7HIW9S1urerHmFajOLjOEl904tp/3PqAHXR3a0RrTog6ta1njKVWnc6I1BSzWnq9w3231hGt7trOTXHdGdNKFRLxz7kPsy/jZbdrS2+m1unN19HV1PGahs43MYOXdK3qpuNWhN/66dSM4S/rF/YiX6r/Sz/tm2aW7ulMd7urduqNS5qxpx/iXmIf1XFPwvqdJ/wAaPL8JVkk3NEV/SA6pVoLcK86dNX5JU8FrWr+KwU60+IW2XjHh0k34Sr04pL9alKmkuZsC5IAAAAAAAAAAAAAAAAAAD13Fvb3lvVtLuhTr0K8JU6tKpFShODXDjJPw00+GmewAU++oX6Zlzt/LIb39OeBr3WmG53Oc01aU3OpiV5cri2ivMrb7yppN0vlc0+fa0/0j+pjvJ04uw0fq2rW1xoC3UaEcZeVv8Xj6S8L8JXfLUYrjilPmHC4j7fPcXxFU3qS+m/C2hkuoXp509204+7e6o05aRSUFw5TvbWmvt8upSj/90Vx3ICxTYrf/AGt6jtDW+v8AarUUMlYTap3VvNe3dWFfjl0Lily3Tmuf6xkvqjKUWpPYp1wek3ql1x0obpWuutL1al1ibpwt8/hnU7aWTtE3zF/aNSHLlTn8xlyvMZSjLsJbVbo6K3o2/wANuZt9l4ZHBZy3Ve3qrxOD54nSqR5+ipCSlCUftKLQHN6i09g9W4HIaY1NirbJYnK21S0vbO5gp0q9GcXGUJJ/KaZRd1z9GOsOjDciz3E23v8AI/uRkb/8RgcrQnKNxh7tNzja1ai8qUeG6c+frjF8/VGRfEY7uHt7o/dbRWX2919g6GXwOct5W17aVl4lF+VKLXmM4ySlGcWpRlFSTTSYEU/T1698T1QaZjoHX9za4/c7CW6dxTTVOnmreK/8VQj9qiSXu018P64/S3GEzjr+dV/S3un0GbyY7UWk83k1gp3rvdI6ot32VYTg+72KziuI14Lw1wo1I/Ulw5Rjad0E9denOrDSC09qWpbYvcrB26llcfFdlO+pJ8fjLZN+YPx3w+YSf+lxbCWoAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPGpTp1qcqVWnGcJxcZRkuVJP5TX3RQB17dN2V6Ruo2dzo38RjtNZyv+8Okby2cqbs3GopTt4T+VO3q9qXDb7JUZN8yOwCaA63OmDHdVOxuT0TShRpamxreT03d1Go+1fQi+KcpfanVi3Tl9l3KXDcEB9XRf1JY7qj2Gwm4aqUYZ62j+zNR2tNKPsZGlFe41H7QqJxqwXniNRL5TN6lBnQZ1LZzo26h7nTu4NK6xmmc1dfsDV9jcRlGWPrUqkoQuZQ+VOhUc1JcN9kqqSb4L76FehdUKdzbVoVaNWCnTqQkpRnFrlNNeGmvuB7AAAAAAAAAAAAAAAAAAAPxpSTjJJprhp/c/QBSd6m/QnW2M1Ncb4bX4qT2+1Bdd2QtKFP6cFe1Jfl4X5bepJ/Q/iMn7fjmn3Yj6avWFnunrdzH7dZ7Je5t7rjI0bPIW9afFPH3lVxp0r6m3+Th9kan2lT8vl04cXjay0hp3cDSeX0Rq3G08hhs7ZVbC+tqi8VaNSLjJf0fD8NeU+GvKOuR1Q9PWqOmPeXN7WakjVq0bWp+JxF/KHbHIY6cn7NdfblpOMkvEZwnHzwB2UARp9PjqOj1IdOGDzmVyCuNU6cisFqFSk3Unc0YrsuJc+X71LsqN/He6iX5WSWAwneXZzQW/W3eW2w3IxCv8Nlqfa3FqNa2qr/AC7ihNp9lWD8xlw18pqUW4ugjevajd7oM6i1i8bqO5s8tgq8cnpvUVnF0lfWkm1TqqD5S5XdTq0pd0eVODc4NSl2LSK3qHdJFLql2Xq/u3aUv370kqmS0/U8KV19P8Wxcn4SqpLtb4SqQpttR7uQ5Hof61NI9XWg5TmrfE67wdKCz2FU/Hnwrq3TfMqEn/3hJ9svmMpyYOsZtZujuJsBuTj9f6FyNfDajwFxKLhVg0pJPtq29em+O6ElzGUHx/2aTXYE6SOqvQ/Vlthb6201KFjmbJQts/hZVVKrjrtx5a/WVGfDdOpwu5Jp8SjKMQ3eAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAACsj1Xeh6tqizuuqHanDuplbCinq/HW8Fzc20I8Rv4RXlzpxSjUXnmCUvHZJy5D0l+s6GtNPUemHcfL85/BW7lpS5rz+q+x9OPMrPl/NShFcwXLbpcrhKl5slqU6danKlVpxnCcXGUZLlST+U190Uy+oJ0Wao6VNwLbqf6fI18fpJZSjftWK+vTOS9zug1HjhWs6nHY39MZS9ppJ0+4LnAaD6Meq3TXVjtHaaws5W9pqbGxp2epcXT5Stbzt8zpqTb9mpw5Qbb4XMW3KLN+AAAAAAAAAAAAAAAAAAAAIr+oT0gWnVVtDOen7alT17pOFW909XfEfxKaTq2M2/5aqiu1vjtqRg+VFz5lQAKEPTa6jrvps6kbbA6qua9jpfWdSOn89QrRlFWtz3tW1xOL8xlTqtwlz+WFWr90i+8pJ9Xbp0t9q98rPdrTWOhb4HcinVuLmNJcRpZek1+J5XxH3Yzp1f+qbrfoWW9Am+tXqC6XtJ6uyd7K6zuKpvAZypN8zne2qjF1JP7yqUpUar/AK1WBIkAAVCerd0bPSWeqdUe3eLn+xs5cRp6ttqMOY2l/N8QvfHxCs2oz8JKrw+W6vChR019Re4HS9ufj9y9CXPco/4fJ46pNq3ydm2nUoVEv7Jxl8xkoyX6Pse6q0tp7W+msno/VmJoZPDZm1qWV/Z11zCvQqRcZwfHlcp/Kaa+U0zr8dUHTEulTf272z1q72rovMP8Thc7Gl3VfwM5cRrJJJVKtCXMatLx3qL47O+nNBe9sbvboLqF21xW6G3WTV1i8lDtqUp8KvZ3EUvct60U/pqQbXK+GnGSbjJN58UHdMXUFuZ6e++UsTq20r3ujs9C2q5iyt599DI4+ou63yljN8Rm+yTnCXhTi5U5dr8wvb0nqvTuutM4zWOkcvbZTDZi2p3ljeW8+6nWpTXMZJ//ANXynyn5QHLAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAB8GfwOF1Vg8hpnUeLtslisrbVLO9s7mmp0rihUi4zpzi/Di4tpr+p94ApV1/pjcb0o+rKx1xoule5TbbUspKlRqSft5DGuadaxqT+FcUeU4Tfn8kmmpTi7htuNw9I7saGwu42hMtTyWBz9rG7s7iH3i21KMl/LOMlKEovzGUZJ+UYl1JdPui+pnabLbWa0oqMLtfiMdfRgnVx19BP2rinz9021JeO6EpxfiTKwuiPqD1p0Ib+5rpR6hJuw0tkMkqLr1pv2cXezS9q8pzk0vwteDh3v4ScJ+O2akFxwAAAAAAAAAAAAAAAAAAAACMnqNbI198+lPVWIxGLqX+f052ajw9KlTc6s69tz7kIRSblKdvKvCMV5cpRIheiTf7iWeT3M05cYG5jo6dGzvJXtanKEaGUjKUFRhyuJOdKUnP5cfZp/Hd5tYAAAACOXXh0s2XVTsXkNNWFtSWsMD35TTFzJqLV3GP1W8pPjinWiux8tJS9ub57EiRoApK6TdMaR6xNtMn0Y7vVp4TcPQ8Lq/2+z1xS/xNpTUn+KxlZPiU6UKj7/af1KMqjj2+0k8l6L+pbcToL3jvuljqXtbnG6Sur7tjUryc4Ye4qP6LuhP4nZ1nw5dvhc+4uGqkZcx6mGzup+mLqK0x1l7QU3YUMxlKVzeSpwftW+cppyl3pcc07mlGTlH+Zqvz+fgltu1shs/6mPTXpvcfDOhitQ3uNd1gM0o99XHXKbVayuGuHUpKtGdOS+zTnHz8hL6hXoXVCnc21aFWjVgp06kJKUZxa5TTXhpr7nsKxugjqo1xsJuHPoZ6qYVsVkMdc/gNMZK+qPtpzbXtWbqS8ToVFw7eovD7owXiUFGzkAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEM/Uj6KKPUzt2tb6ExdH/AGk6UoSlZOK7ZZWyXMp2UmvmXLc6TfxLuj4VRtTMAFdHpY9atzrvDw6ZN28hOlq7TVB0dP3F39FW+s6K4laz7vLr0VHwvmVNPnzBt2LlVnqc9H2e281PDrO2BpXGNurK8p5DUtLHfRUsrtTThlKSX2cuPd45+p+41w6jUv8AoV6wcF1a7U08ndSoWet9Pxp2upcbDhJVWn2XVJf/AAaqi2v9MlOHlRUpBJQAAAAAAAAAAAAAAAAAAAAAAAAAAa76g9ltOdQmz2ptpdTRhC3ztnKnb3Lh3Ss7uP1ULiP9YVFGXHK5ScX4bKnujDqj1l0D7zZ7pk3/ALeVtpWeY9m/fd3rDXsoxUbym0uZ29Wn7UpL/S4ziue5SulK8vVp6QluZoP/AHidC41S1Ro207M3RpR+q/xEW5Op/WdDly/V03Py+yCA2315dGenur/bS21Ho6pZUtf4K1dzpzK06kfbyFvJOf4OpUT4lSqN91OfP0TfcmozqKWvPTq63MzuHKt0y9QVa4x26ek3UsLarkk6dzlqdvzGpSrKXl3dFQanz9U4rvfMlUZpb0oOuKpbXNj0rbqZXuoVm4aMyNefmnP5eOnJ/Z+XRb+HzT8804rdXqL9EuZ3C9nqb6f6d1j909JOne16OM5hc5anQcZU6tLt8/i6KinDj6pxXZ5koICegIl9APW7ieqrQ8tPaqqW+O3K01RjDMWK+hX1JcRV7Rj/AKZPxOC/JN/aMocy0AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPTe2VnkbOvj8haUbq1uqUqNehWpqdOrTkmpQlF+JRabTT8NMpx6kdlNyPTO6hsX1HbDwq1dvcxeSoq0lOcqVCNR99XFXT+9Kai3Sm+Wuxfz01KVyhj+vtB6T3P0Zl9v8AXWFoZbA522laXtpWXMZwflNP5jKMkpRkuHGUYyTTSYGPbDb46F6idsMRunt9fe9jslDtrW82vesbmPHu21aK/LUg3/ZpxkuYyTewSnXE1d0PSQ6lHaZdZHUeyutqzSrQXPv26b7ZpeIRvbdSXdHwqkOeO1SThbrpXVOndb6bxur9JZe2yuGzFtTvLG9t5d1OvRmuYyT/ALP4flPw+GByoAAAAAAAAAAAAAAAAAAAAAAAB4VqNK4pToV6UKlKpFwnCcU4yi1w00/lNHmAOvt1+9M930pdQ11baXp1rPSuoJvO6Wr0ZSi7aHfzO2jLnlSoVPpT557HSk3zItp9Pjqto9Umx1te5y9py1vpX28ZqSlylKrPtfs3nC44jWjFt8JJTjVS8JH56ivTXDqP6c8vZ4bGq41dpJTzun5QhzVqVKcf41rH7v3qSlFR54dSNJv8pT50LdS1z0v9QGG1le3VWOl8rxiNSUYpyUrGrJc1lFfMqU1GouPLUZRX5mBO3r26Tta7F67h1x9KXu4rJYe5eR1PjLGku2k3y6t7GklxOjNOSuKbT8Sc+O1zcZg9H3Vhozq12uo6xwahYZ/HdlrqHDOXM7C7cfmPPmVGfDlTn91ynxKMkt3wnZZOyjUpyoXdpd0k4yTVSnWpyXyvlSi0/wCzTKo+pnZPX/pyb52vVr032Hdt3lbhW+dwce5W9kq0132lRL4tqku10p/8qoox48Q7gtjBgWxu9mhOoTbPEbp7eZH8Ri8rT+ujNpV7K4j/AJltXim+ypB+GvhpqSbjKLeegAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAGAb57H7f8AUPtxktsNyMV+Lxd+u+lVhxGvZXMU1TuKEmn2VIdz4fDTTcWnGTTrn6at2dwfTe3uq9KPUdk/e20z93O403qOpzC1tHUnwrmDk37dvUfCrU+eKNRynzw5ynauad6pemHQHVZthdbfa0pfhb2l3XGEzNKmpXGLvO3iNWK5XfB+FUptpTj94yUZxDcKaklKLTTXKa+5+ldXRN1L7gbDbgf7inVnJWObwrja6Qzlaq50Ly1+KFvGtLj3KUor+BNpNJe1JRlFRjYqAAAAAAAAAAAAAAAAAAAAAAAAAKFvU56Y10+9QN1qDTuOVvo7cB1cxilTX8O3ue5O7tl+ijUmpxS8KFaEV+Vl9JofrW6a7Hqk2FzW30I0qeoLT/imnLmpwlRyNKMuyLk/iFSMp0pP7Kp3cNxQGgfSU6olu1s/V2V1Vkvd1Tt5ShCz92fM7vDNqNGS5fLdGT9mXjhRdDy3Jk4tU6X0/rbTmT0hqvE2+Uw2YtallfWdxHup16NSLjKEv7p/K8r5XDOt5sXu3rfpZ30xG4GPs69tldL5CdrlMZX5pyr0VJ07q0qp/Dce+PlfTJJ8cxR2OdBa307uXonBbg6RvfxeG1Fj6GSsavHDdKrBSipL+WS54lF+YyTT8oCrJUdeekr1IxrOWTz+wW4Fx2yfLk7Z+eOV5Su6C888fx6XK8S/y7WtO6hwercDj9T6ZyttksTlbend2V5bTU6VejOKlGcWvlNMxjenZvQm/m3OX2w3FxSvcTlaTSlHxVtayT9u4oy/lqQb7ov4+zTTade3SnutrzoE31q9GHURkZVND5y4dxozUNWTVtQdapLslFt/RQrT5U48/wAKty39M5TAtBAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABG7rZ6OdN9WGgFStatHE68wEJV9N5vzF06i+r8PVlFOXszfHPHmMuJLnhp6p6AusfUmqcjddKXUlRucLu7o5Ts6Msi1GpmKNJctN/EriEOJNptVafFWLl9bJzkNOv8A6LL3e/HWm9mzFSeH3e0bGFzYXFpNUamVpUn3Roua47a0H5pVG/1g/Ek4BMsETOgvrXtOpnS1xorX0I4fdbSkHQzuNrU1QleKEuyV1SpPhx4lxGpT4XtzfHCUokswAAAAAAAAAAAAAAAAAAAAAAAAKUPWD2Fo7db9Y/dvA45UMPuNaSq3bpwShHLW/bCv4iko+5TlQqefMputL9SY3o/bu09d9MVXby6uvcyW3uUq2Tg2nJWVzKVxQk/PPHfK4guftS4XwbK9R7Yipvx0salx2Ks3cZ7SvGpsRGMO6c6ttGXu0opeW50JVoqK+ZuH6FZfpL71ra7qktdG5O7dLD7i2c8HUUqnbTjexfu2k2vvJyjOjH+twBemaI6xOlLSXVntTc6NyyoWWoceql1p3MSh9Vld9vCjJpOToz4jGpFfKSaXdGJvcAQH6DOrLVuH1JW6LuqGVbF7kaUk7DD319U5eYoU1zCk6j8Tqqnw6c/+bTSfLkn3T4In9enRdQ6ltKW2t9vpxxG7GkIq50/k6Vb2JXSpy9xWlSomlF931U6j49up94xlM4noF61brffGXezm8NtLCbvaOjK3yVpcw9ieTp0n2Srxpy4ca0X4q018P61xGXbAJjAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAr969ukXWWD1TR60ulb8RitxdMT/H5qwx8F3ZOjGPE7iFNeKlXs7lVptP3qbfhyXFSQHRj1eaO6ttsqWosc6OP1ViY07fUeG7vqtrhr/NppvmVCo03CX28xfmLJBFa3WH016+6VNzX1x9JFq7eNrUncay03RpuVtKhN91ev7UWu62nwnVgvNOXFWPak3ALKQal6ZOpPQPVJtfY7j6IuFRqtKhlsVUqKVxjLxL66NTj5X3hPhKcWnwnzFbaAAAAAAAAAAAAAAAAAAAAAAPxpSTjJJprhp/c69PWjs7lek3qzy+P0tGeOsYX9HVWlK1NdqpW1Sq6tJQ/pRrQqUl/+Hk7C5R96weH3Ns+ql5jVzup6VyOItY6Sm/NCFCnSgrqlHjwqiuZVJyT+rtq0m/DiBcLsRurjN8NnNIbsYlU4UtTYqjeVaVN8xoXHHbXo8/8A06sakP7xM8KDukr1I93OlXTNHby105htV6OpXlW8jYXsqlC6oOo05xoXEG1CLknLiVOfmUmvktE6Z/Uk6d+o+6ttNQylXRmrrhqFPC5ycIK5nz+W2uE/brN8riD7aj88QaXIErSBnqD9IGqMrkrXq76a3c4rdPRzje31LHR4rZahSjx7sI/E69OCacOH71PmDUmoxlPMAR36J+r7S3VxtfDPW6oY/V+FjSttSYiMv8iu0+2vST8uhV7ZOLflNSg23HlyIKxOsbY7XXRbvPb9c3TJjVTwdWvxrPA0k/w0VWmvdlKC+Lau+3u4X8Kt2zjxzHsnzsNvloPqK2yxO6W3t+62PyVPitbVHH8RY3Mf8y2rxTfbUg/+zTUotxkmw2EAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAHjUp061OVKrTjOE4uMoyXKkn8pr7o8gBWJ1C7Fbken5u7V6uOlrFzudvchU/9stJUlJ0LWlKTc2oR/LbcvuhJf5E/H+W+1T52I31296i9uMfuZttlld468Xt16E/pr2Nyop1LetH+WpHuXP2aalFuLTeeXtlZ5Gzr4/IWlG6tbqlKjXoVqanTq05JqUJRfiUWm00/DTKzN29qNyPTS3ar9SPT3i7nM7M5+4hT1fpOE5yjjYSl+Zf6YJyl7NZ8+3KXtz5jNKQWcgwzaHd3QW+egMXuXtvmoZLC5Wn3Qlx21KFRcd9GrD+SpB+JR/X4bXDeZgAAAAAAAAAAAAAAAAAAANG9YHStpTq12oq6Czl5LGZWxrO/wAFlYR7nZ3ig4rvj/PSmn2zj+nDXDimbyAHWQ0DbaC0ruasHvvp3MXOAta9zjczQxVwqOQs6iUoe7RcuYOpTqJPtmpRklJcctNbs6hOhDWu1+mKG8+z+chuftJkabu7LUuIpN1bWkpNP8VRXMqajKMououYJx+r25PtOP8AUS28t9s+szcPGwtn+Ay+Rp6goxg+zvje0416qi+HxxVnVj8P8pmelNzeq/02dZ2FjK4Wb0HqGhTv7O1rynXwWesqi71VtZtfwajjUTfZxJNrvjOPCYZL0i+qrunsm7HRW8jvdeaKpuNKFerV7stjqfhL26s3/HhFc8U6j5+FGcUlEuB2d3v2u380hR1xtTq6yzuMm4wrezLitaVXFS9mvSf1UqiTX0yS8cNcpplYuZ6Zulv1DdN325nSXlrHbvc2hB3Ob0Xf8UrWpUbXMlCCftxb+K1GLpttKcITb4hNTuOo3or3cqUadbP7e60xkYqrTU0o3Nu5JpSSbpXVvKUE/wCenJw+7j4Dsg5fEYrUGKvMFnMdbZDHZG3qWt3aXNJVKVejOLjOnOMvEoyi2mn4aZVXnsfrX0nOpGnqbA0sjmen/cS69u5tFN1HYS557E23/iKCbdOUv86l3Rb7k5QkP0V+pjt31GQsdAbkOz0huLNKlToSm42GXn8c205fkqN/8mb7vP0OfniVG7u0+id79vMxtjuFio3+FzVH2qsfCqUpp8wq05fyVISSlGX2aA5vSmqtPa401jNYaTy1vk8NmbWne2N5bz7qdajOPMZJ/wBn8fKfKfk5Yqs6ct19dem9vzddKXUHkJ3G2Wobl3OmNR1E429r7k+I3EW3xCjJvtr0/PtVF3J9rcp2o06lOtTjVpVIzhOKlGUXypJ/DT+6A8gAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA+bJY3H5jH3OJy1jQvbK9ozt7m2uKaqUq1KSalCcX4lFptNPw0z6QBWfuBoHcH0wN1bje7Z7H32oNhNU3cI6q0zTm5Tw05S4jUpdz4Xb3cU6jfD/yqjXMJlhO2m5eiN39EYrcTbrUFtmcDmaKrW11Ql/2lCcX5hUi+YyhJKUZJppNHOZbE4zPYy7wuax9vfY++ozt7q1uKaqUq1KS4lCUX4aabTTK3Nc6J3N9L3cq73e2hx2Q1P0+6mu4z1NppVHOeDqykoxrUnJ/S1yowqPxJJUqj59uaCy4GKbXbo6H3l0Pi9xdus7Qy2Dy1JVKFem/qhL+anUj8wqRfiUX5TMrAAAAAAAAAAAAAAAAAAACDfXh6ceT6tdx9P7l6T3Cx+nL6zx1LC5OhfWc6sKlvCtVqRr03B8uqvelHslwpJR+qPHmRt7007Z6m6f8D07biYijqjT+CwVjhKda6pKFfutbaNCF1Tkm3RrcR5UovldzXLTae1wBRF1UdF+93Qhrq23W2w1FmLrSdveKpidUY9uldYycn9NC7UPyvz2d/Ht1U+OIuTpqRO1HVX08+oRomz2C6x8VjsDr2C9rBanodttG4uJLhSoVWmravLiPdRl/BqtLhc9sFaRmMNiNRYq7wWfxdpksbf0Z293Z3dGNWjXpSXEoThJOMotPhprhlQfXP6V2c0BPI7r9NeOucvpeMZXOR0zByq3uMS8ynbfMrij8vs81IL/WuXEI49W3QxvB0lZyV9lbapnNGVq6jjtT2NGSo8t/RTuI+Xb1v+ltxl57JS4fEkeij1X87oKNhtl1NXd7ndOw7aFlqlKVe/x8fhK6S5lc0l8965qx4fipylHE+kz1NsvojCrZTqlxU9f7dXdBY78Td0Y3N5YW7Xa6dWE0/wAXQS8ds/rivhySjA5nqa9NzA6o0r/vC9DWao620VkKUryrp+zru4ubf7y/Bv8ANUUfiVvP+NBrtSm32xCyHqC2C2d639l7fG3GXsr20u6X7Q01qbGThcO0rOLUatOUXxUpv4nT54kl9pJNQ36VuqLdDo53UpdG3WHdOlh4zjR0xqa5rOVG3oyk40U6zX12k2mozlw6L+mXEU/bg50qdaW8nSFqedLT9aeT01XuP+MaWyM5Rt6sk+2c6f3t66S474r5SU4zSSLK93VsV6p/TReXu1N9bw3H0tbyyOMx952U8ljrpL67SsufqoV0uxVIt0+725c8wcQJ7ggp6VPVNfbu7XXWyWvLmotZ7bUqdtT/ABCca11ik/bpSkn576MkqM+fPHtN8ykydYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAPlyuKxedxl3hc3jbXIY+/oTtru0uqMatG4ozi4zp1ISTjOMk2nFppptM+oAVla70XuZ6Wu5lzu7tNZ3+punvVF5D94tOe851MJWnKMVUg5eE/KjTqt8S4VKq0/bm7DdtNy9Ebv6Jxe4e3eftszgcxS922uaEvv8AEoTj8wnGScZQlw4yTTXg5vNYXEajxF7p/P422yGNyNvUtbu0uaaqUq9GcXGcJxfiUWm00/1Kz9UaZ3G9KndmruFoK0yeqOnTWd/CGXxCqyq1sBWk/Dj3PjvS59uo+FUjFUqklJQqMLPQY7t9uDo7dPR2L1/oDPW2ZwOZoK4s7y3lzGcfhxafmM4tOMoySlGSaaTTRkQAAAAAAAAAAAAAAAAAAAAABCfrL9MfbPqKd9rzbiVporcKrGVWpXp0nHHZWr8/4qnBfRNv5rU13eW5RqPjisPAar6t/Ti3YrWEqF/pm7q1FK5xt5B3GHztCD8SXD7K0eHwqlOSqQ7mlKDbR2FDCN4Nl9td99F3mgt0NLWeZxd1CSg6tOPvWlRxaVa3qcd1KqufE48P7PlNphW7S0B04eq1pbJav0Vb2u1+/OJoe7lbSKU7bJ+IJXFVRSdak5Ps95JVab4U1Uiod0DNT6R6hui7d2hDJ0szobWGIk61jfW1T+Hc0uePco1FzTr0ZfDXmL8xmueYmxN/thd7/Tz33sNQ6azN9b2tvdzutKaoto8Qu6P3pVVx2qooS7KtKS7ZJy47oS5LC9m+p/pb9RnbGltD1CYjDYvWyp9ksdd1lQlUuOOFdYu5lxJTfCbpp968xcakOWwrJ0V1Yar0N1NWPU5gMPZ43MV71Xmfx1gvas8h7v03sYwfPZGuu6bT5UKs3KPHbFLsG7Z7iaZ3a2/wG5WjruVxhtR2FK/tJySU4xmuXCaXPbOL5jJfaUWvsUfdZfpv7o9ME7zWmmZV9YbdRqOSytGj/isbBv6Y3tKP5UuVH3o/w2+OVTclAz/oI9TbIbD4/G7N72U62U2/tm6ONylCk53mEhKTk4yjFc3FBSk32/5kE2o90VGmguoBxOldV6a1zp2w1do7O2WZwuUoq4s76yrRq0a9N/eMl4flNNfKaafDTOWAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABxep9M6f1pp3JaS1XibbKYfL21SzvrO4h3U69GcXGUJL9Gn/dfY5QAVg3tDcP0od4VkcbDK6n6a9c3/ABXt+ZVauAuZ8eU38VYxX0t8KvTj2v64KUbKNJ6s01rrTeO1ho7N2mYwuWoRurK+tKinSr05fEotf9018ppp8NNHr1pozS+4elcpojWmFtstg8zbytb6zuI8wq05fb9U0+GmuGmk000mVu4XJ7j+lLu3HS+o6mV1T03a1vnKxyHbKrW0/cTb5UkvCqJeZxXCrQj3wSnGcALPAcfp/UGD1Zg7DU2mctaZTE5S3hd2V7aVVUo3FGa5jOEl4aaafJyAAAAAAAAAAAAAAAAAAAAAABh27W0e32+Ohchtzubp2hmMJkUnOlU5jOjUXPZWpTX1U6keXxKLT8tfDadQXUV6Qm+W3l9fZvZKvQ3B01GU6tG0VSFvl7ekvPbOlPinWaXhOlLum1yqceeC64AddKz6uOqzbbQWq+nzNa2ztPC5ayrYTJYfUFGVW5sKU49lWjSdde7b8wcoOHKjxJ/Snw1tfZv0xdzt8+l+2330VqGzWeyVxc1MXp+6SpxvrOjUlSbVZvinVdSnPtU12yTXMoLy7cN9+j7p56krqzyW7O3ttksnYR9ujkravUtLt0/PFKdWjKMqkE22oybSbbXHL52bo3R+mdvtK4rRGjcRRxeDwlrTsrCzotuNGjBcRjzJuUn+rk22+W222wKFOmnq1346DtxL/R+Zw2RnhKd52ah0blu+h21FwpVaPcn7Fbt4+tJxmlHuUkotXd7CdQm13UloShr/AGtz0b20k1TvLSrxC7x9fjl0biny+ya/u4yXmLkuGYZ1U9F2znVjp52us8b+zNS2lJwxmpbClFXtq/5YT58V6PPzSm/u+1wk+4qH1Vt91X+mHvHa6qx1zKjZ16roWeYtoSq4fPW6+p29eD44k4p80p8Ti05QfiNQC/QEeej3rS226udHu9wc4YfV2MpQea07Xqp1reT4Tq0X/wA2g5eFNLleFJRbXMhgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAY7uFt7o3dXRuU0Br/A22ZwOZouheWddPtnHnlNNeYyi0pRlFpxaTTTRkQArO0lqbcX0st0qG2241/kdTdOWrr2csHnZU51a2n7mf1OnNR/Lxw3OnFcVFzVppTVWmWS4fM4jUWJs89gMpaZLG5GhC6tLy0rRq0bijOKlCpTnFuMotNNNPhpnD7ibd6M3X0ZlNv9wMDbZjBZii6F1a14+GvtKL+Yzi+JRkuHFpNNNFfmktUbi+lxuTbba7l5DJ6o6cdT3k1g9QujOtX03VnJy9urGC+E23OEV9a5q0l3KdJhZOD5cVlcXncXZ5vCZK1yGOyFCndWl3a1o1aFxQqRUoVKc4txnCUWmpJtNNNH1AAAAAAAAAAAAAAAAAAAAAAAAADg9a6H0huPpi+0ZrvTlhncJkqftXVje0VUpVF9nw/hp+VJcNNJpprk5wAVAdT/AKdu7nSvq1dQ/R9mszdYvD15X/4G1bq5TCx+Zdq4f4u2S7k005KHiaqLumS46GvUP0Z1QY+30NraNrpvc21pfxrHu7LbKqK+qraOT5UvHMqLblH5Tkk2pjkFusb01MDuvk6m8fTze0NC7m2dVX/FrN2tpkriD7lU7qfm3uOVyqsVxKXmS5bmgnSCCXR5156iv9Sx6aOr7G1dIbqY2cbS1vchSVvSzL+IKfH0Qry+0ov26vKcOG0nO0AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAGO7gbf6P3S0hk9B69wVtmMHlqLo3VrcQ5jJfaSfzGSfDUl5TSaMiAFb+jtWa79MDdGy2m3My99qDpz1fe1HpzO1YupV0zdVJOUqM+OWqfLcpwXhputTSn70JWM2N9ZZOyt8ljbyhd2l3ShXt7ihUVSnWpySlGcJR5UotNNNeGmY5uhthojeTQ2V263EwdHK4PL0var0KnhxfzGpCXzCcXxKMl5TRArZ3c7Xnpy7qWfTJ1CZyvl9odRVpS0NrKsmqeNTk+aFdv8kE3FThzxTclNfw5toLHweFGtSuKUK9CrCpSqRU4ThJOMotcppr5TR5gAAAAAAAAAAAAAAAAAAAAAAAAAABqzevph2P6hamHud19C2uXu8FcQuLG8hUnb3NPiXLpurScZypSa8wbcX88cpM2mAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAANf76bHbf9Q+3GS2y3HxSu8bfx76NaCSr2Vyk1TuKMmvpqQ5fD+Gm4tOLaewABXR0777bh9EO6Fp0d9WGWdxpK9l26A1vWb/Du3c+2FCtUk/ppJtR+p80JNRk/acJxsXNTdTXTZoDqk2wvduNc0PZqPmvisrSpRlcYu7S+mtT5+V9pw5SnFtcp8SUUejzqT3A2C3GpdDHVtWVrmsd2W2itSVqj/D5O0fMbeh7kku+Mu3tozfnlezJKcUmFg4AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABH/rK6R9JdWO2zwd5KnjNXYRVLrTOcS4nZ3LSftza+p0KjjFTS+OIyX1RRIAAQc6Fer3VuS1DedI3VBCrh929JSlZ2Ve94i85b0ocr6vipWjTXepptVqbVRNtSbnGRM68OjGPUTp+y3H20uXg93NGKN1gcpb1HRqXcaUvcjazqRacZKf1UqnzCf6KUj4OhPrlst/MZPafdmK07vBpmMrXJY67pu3eTVJqMq9OEku2qn4qUflNOUV28qITCAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAIm9Z3Qjheol0dzNtcwtFbuYXtrY7P2s5W/4ydOKVOnc1KS9xOPbFQrR5nBLhKS8EsgBBjo+68dTZnW9Tpd6vMX+6W7uLrqwtrq5pQoUM1V4+mD7P4UK81xKDpv2q6knT4coRlOcjZ1p9FGhurXRqnL2cJr3C0ZPA6ghD6ovnu/DXHHmpQlL/AM1OTcofM4z0n0Q9ZuusVru46OOrl1cbuPg637Pw+Wvanc8v2r6aFWp8TquPEqdblqvFrz38OoE/wAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAACG/qQdHkuobbqG4+31pOjudoWjK6xVW25hWyNrB+5O07o/U6iac6L+1TmK4VSUlMgARN9Orq+XVHtE7DVl3D/aBo9U7LOwaUZXtNpqjfRivCU1Fxml8VIS8KMoIlkVL9YGgta+n71WYnq+2ax9WejNX3s1nMfD6beNzVk53djPhcQp14xdak2n21Iy4XFOKdm+0W7Gid8Nu8Nudt7lY3+FzdBVqUvCqUZrxOjVj/AC1ISTjKP2afyuGwzEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAGI7s7V6L3s28ze2G4OMV9g87bu3uIJpVKcuU4Vacmn21ITUZxlw+JRXh/BWZ0f6Z6leiLrGq9NN7gMrqTb/AFfdykr2jbVPwboKLdLJwkuYUaijGMK1Ny/6eZdtOTthAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAf//Z</t>
         </is>
       </c>
     </row>

</xml_diff>